<commit_message>
Updated config for dev to test convert Removed default events.json Updated excel_to_json.py to handle Unicode Updated index.html to map new Excel structure Updated Excel structure to include Images
</commit_message>
<xml_diff>
--- a/WCS.xlsx
+++ b/WCS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/96c3b0ae7c2036b9/Projects/TDS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\git\westie-agenda\westie-agenda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1807" documentId="11_7D4755BF84DCCE13E97046798E31F45B5A712953" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADFA9D63-FF53-426D-9FC7-2D092760999E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59237C78-FAF2-49BE-8F33-E60AD6C1036D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="767" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="767" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="How To" sheetId="19" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="282">
   <si>
     <t>Faire le Sondage</t>
   </si>
@@ -867,6 +867,30 @@
   </si>
   <si>
     <t>Date Début</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>TDS-Mardi-Ete-Tile.svg</t>
+  </si>
+  <si>
+    <t>TDS-Jeudi-Ete-Tile.svg</t>
+  </si>
+  <si>
+    <t>TDS-StageEteDeb-Tile.svg</t>
+  </si>
+  <si>
+    <t>TDS-StageEteInter-Tile.svg</t>
+  </si>
+  <si>
+    <t>FAC-Vendredi-Tile.svg</t>
+  </si>
+  <si>
+    <t>LSD-Dimanche-Generic-Tile.svg</t>
+  </si>
+  <si>
+    <t>EVT-WOTP2024-Tile.svg</t>
   </si>
 </sst>
 </file>
@@ -1104,6 +1128,20 @@
   </cellStyles>
   <dxfs count="42">
     <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1120,14 +1158,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1173,14 +1203,6 @@
       <alignment horizontal="left"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left"/>
     </dxf>
     <dxf>
@@ -1595,10 +1617,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB0A8277-F879-405D-BC41-C411DB022892}" name="Tableau1" displayName="Tableau1" ref="A1:C25" totalsRowShown="0">
   <autoFilter ref="A1:C25" xr:uid="{AB0A8277-F879-405D-BC41-C411DB022892}"/>
@@ -1642,7 +1660,7 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{C299B888-6182-43CD-96F9-426BE7578FFF}" name="TBL_FULL" displayName="TBL_FULL" ref="A1:J128" totalsRowShown="0" dataDxfId="26">
   <autoFilter ref="A1:J128" xr:uid="{C299B888-6182-43CD-96F9-426BE7578FFF}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J93">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I93">
     <sortCondition ref="A1:A93"/>
   </sortState>
   <tableColumns count="10">
@@ -1656,55 +1674,51 @@
     <tableColumn id="6" xr3:uid="{7281A423-F84C-4A96-B4AF-F2A866B96E9A}" name="Sondage" dataDxfId="18">
       <calculatedColumnFormula>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{450ABC29-053E-4F29-B781-69081341FCE3}" name="Infos" dataDxfId="17">
-      <calculatedColumnFormula>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{52F64AB4-B550-4EE3-A161-F4F84BAC2A77}" name="Infos + Lien" dataDxfId="2">
+      <calculatedColumnFormula>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{52F64AB4-B550-4EE3-A161-F4F84BAC2A77}" name="Infos + Lien" dataDxfId="16">
-      <calculatedColumnFormula>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="7" xr3:uid="{C3C24A01-F990-49C0-96AD-9589DEF3C1DF}" name="Image" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9E08D3BB-8A20-476F-8B56-C00EF44E04B9}" name="TblLatest" displayName="TblLatest" ref="A1:N8" totalsRowShown="0" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9E08D3BB-8A20-476F-8B56-C00EF44E04B9}" name="TblLatest" displayName="TblLatest" ref="A1:N8" totalsRowShown="0" dataDxfId="17">
   <autoFilter ref="A1:N8" xr:uid="{BD7D0BFF-D107-431C-8453-3E1280F0D854}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N6">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M6">
     <sortCondition ref="A1:A6"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{5A32B7B5-F113-4E8A-B61F-4A6A3A219F38}" name="Date Début" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{5939C56E-1752-414F-9B1F-26915CA547CB}" name="Heure Début" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{C842EEE1-6786-415B-92F1-90A15F629A93}" name="Date Fin" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{276A4F50-4151-4619-9D28-3B323183A070}" name="Heure Fin" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{7D76EA45-6B9F-47AA-BC4B-333C0A217D3B}" name="Jour" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{5A32B7B5-F113-4E8A-B61F-4A6A3A219F38}" name="Date Début" dataDxfId="16"/>
+    <tableColumn id="13" xr3:uid="{5939C56E-1752-414F-9B1F-26915CA547CB}" name="Heure Début" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{C842EEE1-6786-415B-92F1-90A15F629A93}" name="Date Fin" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{276A4F50-4151-4619-9D28-3B323183A070}" name="Heure Fin" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{7D76EA45-6B9F-47AA-BC4B-333C0A217D3B}" name="Jour" dataDxfId="12">
       <calculatedColumnFormula>VLOOKUP(PROPER(TEXT(A2,"dddd")),TblDays[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F991CC75-7E43-4E27-BAC1-A13A0DDB4EA2}" name="Type" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{116FD67B-CB4E-4768-8852-B3B7D0487065}" name="Lieu / Ecole" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{4ADFCFB0-CAC8-47AB-B266-B6AB9CB80AAA}" name="Nom" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{D62EB0AF-952F-419A-BDDA-B2803683F3C7}" name="Nom Court" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{A105BFB5-86A5-4432-8027-0B0690E84654}" name="URL" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{13903E95-80BF-4327-8073-66A5B7170295}" name="Sondage" dataDxfId="4">
+    <tableColumn id="3" xr3:uid="{F991CC75-7E43-4E27-BAC1-A13A0DDB4EA2}" name="Type" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{116FD67B-CB4E-4768-8852-B3B7D0487065}" name="Lieu / Ecole" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{4ADFCFB0-CAC8-47AB-B266-B6AB9CB80AAA}" name="Nom" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{D62EB0AF-952F-419A-BDDA-B2803683F3C7}" name="Nom Court" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{A105BFB5-86A5-4432-8027-0B0690E84654}" name="URL" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{13903E95-80BF-4327-8073-66A5B7170295}" name="Sondage" dataDxfId="6">
       <calculatedColumnFormula>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{B7FBBB4C-03E9-4318-B4BF-37524775C9CB}" name="Calendrier" dataDxfId="3">
+    <tableColumn id="14" xr3:uid="{B7FBBB4C-03E9-4318-B4BF-37524775C9CB}" name="Calendrier" dataDxfId="5">
       <calculatedColumnFormula>IF(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]], "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2D02E16D-E492-4F70-8F08-4957F4B3D549}" name="Infos" dataDxfId="2">
-      <calculatedColumnFormula>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]]</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{9EE3ABE6-B859-41C5-A834-29D644768C27}" name="Infos + Lien" dataDxfId="3">
+      <calculatedColumnFormula>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9EE3ABE6-B859-41C5-A834-29D644768C27}" name="Infos + Lien" dataDxfId="1">
-      <calculatedColumnFormula>TblLatest[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="7" xr3:uid="{3CCCE9DB-4FCC-4478-A1DC-9C0D98780478}" name="Image" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D74DDD-8432-4192-A172-BF3ECD73FB3B}" name="TblDays" displayName="TblDays" ref="A1:B8" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D74DDD-8432-4192-A172-BF3ECD73FB3B}" name="TblDays" displayName="TblDays" ref="A1:B8" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:B8" xr:uid="{13D74DDD-8432-4192-A172-BF3ECD73FB3B}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{72BE85DD-EFE9-4638-8C61-73698AE82F8A}" name="Day"/>
@@ -2466,7 +2480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53D23E2-73CD-48EF-BF16-8F4C63AFD3E5}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -3458,8 +3472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB9F931-09B4-4724-BB11-DDCAA6AA5863}">
   <dimension ref="A1:J128"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView topLeftCell="C106" workbookViewId="0">
+      <selection activeCell="I136" sqref="I136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3472,8 +3486,8 @@
     <col min="6" max="6" width="26.42578125" customWidth="1"/>
     <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="36.85546875" customWidth="1"/>
-    <col min="9" max="9" width="49.5703125" customWidth="1"/>
-    <col min="10" max="10" width="60.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -3502,10 +3516,10 @@
         <v>68</v>
       </c>
       <c r="I1" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
       <c r="J1" t="s">
-        <v>130</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -3534,14 +3548,11 @@
         <v>Mar. 🪩 After TDS</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mar. TDS - After Mardi</v>
-      </c>
-      <c r="J2" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v xml:space="preserve">Mar. TDS - After Mardi_x000D_
 &gt; </v>
       </c>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
@@ -3549,7 +3560,7 @@
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" ref="B3:B8" si="0">PROPER(TEXT(A3,"jjjj"))</f>
-        <v>Jeudi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>88</v>
@@ -3566,17 +3577,14 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Jeu. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I3" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Jeu. TDS - After Jeudi</v>
-      </c>
-      <c r="J3" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v xml:space="preserve">Jeu. TDS - After Jeudi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v xml:space="preserve">Jjj. TDS - After Jeudi_x000D_
 &gt; </v>
       </c>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
@@ -3584,7 +3592,7 @@
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>88</v>
@@ -3601,17 +3609,14 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Soirée Factory Club</v>
+        <v>Jjj. 🪩 Soirée Factory Club</v>
       </c>
       <c r="I4" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Factory Club - Soirée RWSB</v>
-      </c>
-      <c r="J4" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v xml:space="preserve">Ven. Factory Club - Soirée RWSB_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v xml:space="preserve">Jjj. Factory Club - Soirée RWSB_x000D_
 &gt; </v>
       </c>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -3619,7 +3624,7 @@
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>88</v>
@@ -3636,17 +3641,14 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Soirée MTG (R4T + WCS)</v>
+        <v>Jjj. 🪩 Soirée MTG (R4T + WCS)</v>
       </c>
       <c r="I5" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Rock4U - Move That Gallery</v>
-      </c>
-      <c r="J5" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v xml:space="preserve">Ven. Rock4U - Move That Gallery_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v xml:space="preserve">Jjj. Rock4U - Move That Gallery_x000D_
 &gt; </v>
       </c>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
@@ -3654,7 +3656,7 @@
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Samedi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>73</v>
@@ -3674,14 +3676,11 @@
         <v>WE 🎟️ Stage "Les Virginies"</v>
       </c>
       <c r="I6" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. Friendly Danses - Stage "Les Virginies"</v>
-      </c>
-      <c r="J6" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v xml:space="preserve">Sam. Friendly Danses - Stage "Les Virginies"_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v xml:space="preserve">WE. Friendly Danses - Stage "Les Virginies"_x000D_
 &gt; </v>
       </c>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -3689,7 +3688,7 @@
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>88</v>
@@ -3706,17 +3705,14 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 🪩 Happy Sunday</v>
+        <v>Jjj. 🪩 Happy Sunday</v>
       </c>
       <c r="I7" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. La Station - Happy Sunday</v>
-      </c>
-      <c r="J7" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v xml:space="preserve">Dim. La Station - Happy Sunday_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v xml:space="preserve">Jjj. La Station - Happy Sunday_x000D_
 &gt; </v>
       </c>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
@@ -3724,7 +3720,7 @@
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Mardi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>88</v>
@@ -3741,17 +3737,14 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Mar. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I8" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mar. TDS - After Mardi</v>
-      </c>
-      <c r="J8" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v xml:space="preserve">Mar. TDS - After Mardi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v xml:space="preserve">Jjj. TDS - After Mardi_x000D_
 &gt; </v>
       </c>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
@@ -3778,14 +3771,11 @@
         <v>Jeu. 🪩 After TDS</v>
       </c>
       <c r="I9" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Jeu. TDS - After Jeudi</v>
-      </c>
-      <c r="J9" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v xml:space="preserve">Jeu. TDS - After Jeudi_x000D_
 &gt; </v>
       </c>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
@@ -3793,7 +3783,7 @@
       </c>
       <c r="B10" s="1" t="str">
         <f>PROPER(TEXT(A10,"jjjj"))</f>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>88</v>
@@ -3810,17 +3800,14 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Soirée Factory Club</v>
+        <v>Jjj. 🪩 Soirée Factory Club</v>
       </c>
       <c r="I10" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Factory Club - Soirée RWSB</v>
-      </c>
-      <c r="J10" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v xml:space="preserve">Ven. Factory Club - Soirée RWSB_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v xml:space="preserve">Jjj. Factory Club - Soirée RWSB_x000D_
 &gt; </v>
       </c>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
@@ -3828,7 +3815,7 @@
       </c>
       <c r="B11" s="1" t="str">
         <f>PROPER(TEXT(A11,"jjjj"))</f>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>73</v>
@@ -3848,14 +3835,11 @@
         <v>WE 🎟️ West In Champagne</v>
       </c>
       <c r="I11" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. WCSC - West In Champagne</v>
-      </c>
-      <c r="J11" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v xml:space="preserve">Ven. WCSC - West In Champagne_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v xml:space="preserve">WE. WCSC - West In Champagne_x000D_
 &gt; </v>
       </c>
+      <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
@@ -3863,7 +3847,7 @@
       </c>
       <c r="B12" s="1" t="str">
         <f>PROPER(TEXT(A12,"jjjj"))</f>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>88</v>
@@ -3880,17 +3864,14 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 🪩 Dimanche WCS</v>
+        <v>Jjj. 🪩 Dimanche WCS</v>
       </c>
       <c r="I12" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. DK'Danse - Dimanche WCS</v>
-      </c>
-      <c r="J12" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v xml:space="preserve">Dim. DK'Danse - Dimanche WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v xml:space="preserve">Jjj. DK'Danse - Dimanche WCS_x000D_
 &gt; </v>
       </c>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
@@ -3898,7 +3879,7 @@
       </c>
       <c r="B13" s="1" t="str">
         <f>PROPER(TEXT(A13,"jjjj"))</f>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>88</v>
@@ -3915,17 +3896,14 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 🪩 Happy Sunday</v>
+        <v>Jjj. 🪩 Happy Sunday</v>
       </c>
       <c r="I13" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. La Station - Happy Sunday</v>
-      </c>
-      <c r="J13" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v xml:space="preserve">Dim. La Station - Happy Sunday_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v xml:space="preserve">Jjj. La Station - Happy Sunday_x000D_
 &gt; </v>
       </c>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
@@ -3933,7 +3911,7 @@
       </c>
       <c r="B14" s="1" t="str">
         <f>PROPER(TEXT(A14,"jjjj"))</f>
-        <v>Mardi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>88</v>
@@ -3950,17 +3928,14 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Mar. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I14" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mar. TDS - After Mardi</v>
-      </c>
-      <c r="J14" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v xml:space="preserve">Mar. TDS - After Mardi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v xml:space="preserve">Jjj. TDS - After Mardi_x000D_
 &gt; </v>
       </c>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
@@ -3987,14 +3962,11 @@
         <v>Jeu. 🪩 After TDS</v>
       </c>
       <c r="I15" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Jeu. TDS - After Jeudi</v>
-      </c>
-      <c r="J15" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v xml:space="preserve">Jeu. TDS - After Jeudi_x000D_
 &gt; </v>
       </c>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
@@ -4002,7 +3974,7 @@
       </c>
       <c r="B16" s="1" t="str">
         <f>PROPER(TEXT(A16,"jjjj"))</f>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>88</v>
@@ -4019,17 +3991,14 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Soirée Factory Club</v>
+        <v>Jjj. 🪩 Soirée Factory Club</v>
       </c>
       <c r="I16" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Factory Club - Soirée RWSB</v>
-      </c>
-      <c r="J16" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v xml:space="preserve">Ven. Factory Club - Soirée RWSB_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v xml:space="preserve">Jjj. Factory Club - Soirée RWSB_x000D_
 &gt; </v>
       </c>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
@@ -4037,7 +4006,7 @@
       </c>
       <c r="B17" s="1" t="str">
         <f>PROPER(TEXT(A17,"jjjj"))</f>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>88</v>
@@ -4054,17 +4023,14 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Level Up You WCS</v>
+        <v>Jjj. 🪩 Level Up You WCS</v>
       </c>
       <c r="I17" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Studio Diabolo - Level Up You WCS</v>
-      </c>
-      <c r="J17" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v xml:space="preserve">Ven. Studio Diabolo - Level Up You WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v xml:space="preserve">Jjj. Studio Diabolo - Level Up You WCS_x000D_
 &gt; </v>
       </c>
+      <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
@@ -4091,14 +4057,11 @@
         <v>Sam. 🪩 Soirée TDS</v>
       </c>
       <c r="I18" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. TDS - Soirée</v>
-      </c>
-      <c r="J18" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v xml:space="preserve">Sam. TDS - Soirée_x000D_
 &gt; </v>
       </c>
+      <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
@@ -4125,14 +4088,11 @@
         <v>Sam. 📚 Styling Follower</v>
       </c>
       <c r="I19" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. TDS - Styling Follower TDS</v>
-      </c>
-      <c r="J19" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v xml:space="preserve">Sam. TDS - Styling Follower TDS_x000D_
 &gt; </v>
       </c>
+      <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
@@ -4140,7 +4100,7 @@
       </c>
       <c r="B20" s="1" t="str">
         <f>PROPER(TEXT(A20,"jjjj"))</f>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>120</v>
@@ -4157,17 +4117,14 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 📚 Stage WCS</v>
+        <v>Jjj. 📚 Stage WCS</v>
       </c>
       <c r="I20" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. TDS - Stage WCS</v>
-      </c>
-      <c r="J20" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v xml:space="preserve">Dim. TDS - Stage WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v xml:space="preserve">Jjj. TDS - Stage WCS_x000D_
 &gt; </v>
       </c>
+      <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
@@ -4175,7 +4132,7 @@
       </c>
       <c r="B21" s="1" t="str">
         <f>PROPER(TEXT(A21,"jjjj"))</f>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>88</v>
@@ -4192,17 +4149,14 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 🪩 Happy Sunday</v>
+        <v>Jjj. 🪩 Happy Sunday</v>
       </c>
       <c r="I21" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. La Station - Happy Sunday</v>
-      </c>
-      <c r="J21" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v xml:space="preserve">Dim. La Station - Happy Sunday_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v xml:space="preserve">Jjj. La Station - Happy Sunday_x000D_
 &gt; </v>
       </c>
+      <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
@@ -4210,7 +4164,7 @@
       </c>
       <c r="B22" s="1" t="str">
         <f>PROPER(TEXT(A22,"jjjj"))</f>
-        <v>Mardi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>88</v>
@@ -4229,17 +4183,14 @@
       </c>
       <c r="H22" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Mar. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I22" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mar. TDS - After Mardi</v>
-      </c>
-      <c r="J22" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Mar. TDS - After Mardi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Mardi_x000D_
 &gt; https://vu.fr/AYWaj</v>
       </c>
+      <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
@@ -4268,14 +4219,11 @@
         <v>Jeu. 🪩 After TDS</v>
       </c>
       <c r="I23" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Jeu. TDS - After Jeudi</v>
-      </c>
-      <c r="J23" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v>Jeu. TDS - After Jeudi_x000D_
 &gt; https://vu.fr/MFGS</v>
       </c>
+      <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
@@ -4283,7 +4231,7 @@
       </c>
       <c r="B24" s="1" t="str">
         <f>PROPER(TEXT(A24,"jjjj"))</f>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>88</v>
@@ -4302,17 +4250,14 @@
       </c>
       <c r="H24" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Soirée Factory Club</v>
+        <v>Jjj. 🪩 Soirée Factory Club</v>
       </c>
       <c r="I24" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Factory Club - Soirée RWSB</v>
-      </c>
-      <c r="J24" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Factory Club - Soirée RWSB_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Factory Club - Soirée RWSB_x000D_
 &gt; https://vu.fr/fPBPm</v>
       </c>
+      <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
@@ -4341,14 +4286,11 @@
         <v>Ven. 🪩 La MAS</v>
       </c>
       <c r="I25" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. La MAS - La MAS WCS</v>
-      </c>
-      <c r="J25" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v>Ven. La MAS - La MAS WCS_x000D_
 &gt; https://vu.fr/eWqLx</v>
       </c>
+      <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
@@ -4356,7 +4298,7 @@
       </c>
       <c r="B26" s="1" t="str">
         <f>PROPER(TEXT(A26,"jjjj"))</f>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>73</v>
@@ -4378,14 +4320,11 @@
         <v>WE 🎟️ Westy Nantes</v>
       </c>
       <c r="I26" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. WSDC - Westy Nantes</v>
-      </c>
-      <c r="J26" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. WSDC - Westy Nantes_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>WE. WSDC - Westy Nantes_x000D_
 &gt; https://vu.fr/wkCI</v>
       </c>
+      <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
@@ -4393,7 +4332,7 @@
       </c>
       <c r="B27" s="1" t="str">
         <f>PROPER(TEXT(A27,"jjjj"))</f>
-        <v>Mardi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>88</v>
@@ -4412,17 +4351,14 @@
       </c>
       <c r="H27" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Mar. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I27" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mar. TDS - After Mardi</v>
-      </c>
-      <c r="J27" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Mar. TDS - After Mardi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Mardi_x000D_
 &gt; https://vu.fr/JydaD</v>
       </c>
+      <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
@@ -4451,14 +4387,11 @@
         <v>Jeu. 🪩 After TDS</v>
       </c>
       <c r="I28" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Jeu. TDS - After Jeudi</v>
-      </c>
-      <c r="J28" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v>Jeu. TDS - After Jeudi_x000D_
 &gt; https://vu.fr/cvhZg</v>
       </c>
+      <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
@@ -4466,7 +4399,7 @@
       </c>
       <c r="B29" s="1" t="str">
         <f>PROPER(TEXT(A29,"jjjj"))</f>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>88</v>
@@ -4485,17 +4418,14 @@
       </c>
       <c r="H29" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Soirée Factory Club</v>
+        <v>Jjj. 🪩 Soirée Factory Club</v>
       </c>
       <c r="I29" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Factory Club - Soirée RWSB</v>
-      </c>
-      <c r="J29" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Factory Club - Soirée RWSB_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Factory Club - Soirée RWSB_x000D_
 &gt; https://vu.fr/fPBPm</v>
       </c>
+      <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
@@ -4524,14 +4454,11 @@
         <v>Ven. 🪩 West In Palaiseau</v>
       </c>
       <c r="I30" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Belle Fee Danse - West In Palaiseau</v>
-      </c>
-      <c r="J30" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v>Ven. Belle Fee Danse - West In Palaiseau_x000D_
 &gt; https://vu.fr/Gucy</v>
       </c>
+      <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
@@ -4539,7 +4466,7 @@
       </c>
       <c r="B31" s="1" t="str">
         <f>PROPER(TEXT(A31,"jjjj"))</f>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>88</v>
@@ -4558,17 +4485,14 @@
       </c>
       <c r="H31" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 WCS Olympiade</v>
+        <v>Jjj. 🪩 WCS Olympiade</v>
       </c>
       <c r="I31" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Sensation Danse - Soirée WCS Olympiade</v>
-      </c>
-      <c r="J31" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Sensation Danse - Soirée WCS Olympiade_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Sensation Danse - Soirée WCS Olympiade_x000D_
 &gt; https://vu.fr/wLcXW</v>
       </c>
+      <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
@@ -4576,7 +4500,7 @@
       </c>
       <c r="B32" s="1" t="str">
         <f>PROPER(TEXT(A32,"jjjj"))</f>
-        <v>Samedi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>88</v>
@@ -4595,17 +4519,14 @@
       </c>
       <c r="H32" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Sam. 🪩 La MAS</v>
+        <v>Jjj. 🪩 La MAS</v>
       </c>
       <c r="I32" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. Connexion Swing - La MAS WCS</v>
-      </c>
-      <c r="J32" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Sam. Connexion Swing - La MAS WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Connexion Swing - La MAS WCS_x000D_
 &gt; https://vu.fr/TtsFI</v>
       </c>
+      <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
@@ -4613,7 +4534,7 @@
       </c>
       <c r="B33" s="1" t="str">
         <f>PROPER(TEXT(A33,"jjjj"))</f>
-        <v>Samedi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>88</v>
@@ -4632,17 +4553,14 @@
       </c>
       <c r="H33" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Sam. 🪩 Soirée WCS SDC</v>
+        <v>Jjj. 🪩 Soirée WCS SDC</v>
       </c>
       <c r="I33" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. Social Danse Club - Soirée WCS SDC</v>
-      </c>
-      <c r="J33" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Sam. Social Danse Club - Soirée WCS SDC_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Social Danse Club - Soirée WCS SDC_x000D_
 &gt; https://vu.fr/Clxhc</v>
       </c>
+      <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
@@ -4650,7 +4568,7 @@
       </c>
       <c r="B34" s="1" t="str">
         <f>PROPER(TEXT(A34,"jjjj"))</f>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>88</v>
@@ -4669,17 +4587,14 @@
       </c>
       <c r="H34" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 🪩 Happy Sunday</v>
+        <v>Jjj. 🪩 Happy Sunday</v>
       </c>
       <c r="I34" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. La Station - Happy Sunday</v>
-      </c>
-      <c r="J34" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Dim. La Station - Happy Sunday_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. La Station - Happy Sunday_x000D_
 &gt; http://station-danse.fr/</v>
       </c>
+      <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
@@ -4687,7 +4602,7 @@
       </c>
       <c r="B35" s="1" t="str">
         <f>PROPER(TEXT(A35,"jjjj"))</f>
-        <v>Mardi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>88</v>
@@ -4706,17 +4621,14 @@
       </c>
       <c r="H35" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Mar. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I35" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mar. TDS - After Mardi</v>
-      </c>
-      <c r="J35" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Mar. TDS - After Mardi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Mardi_x000D_
 &gt; https://vu.fr/yRkaN</v>
       </c>
+      <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
@@ -4745,14 +4657,11 @@
         <v>Jeu. 🪩 After TDS</v>
       </c>
       <c r="I36" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Jeu. TDS - After Jeudi</v>
-      </c>
-      <c r="J36" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v>Jeu. TDS - After Jeudi_x000D_
 &gt; https://vu.fr/FHWLc</v>
       </c>
+      <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
@@ -4760,7 +4669,7 @@
       </c>
       <c r="B37" s="1" t="str">
         <f t="shared" ref="B37:B42" si="1">PROPER(TEXT(A37,"jjjj"))</f>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>88</v>
@@ -4779,17 +4688,14 @@
       </c>
       <c r="H37" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Soirée Factory Club</v>
+        <v>Jjj. 🪩 Soirée Factory Club</v>
       </c>
       <c r="I37" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Factory Club - Soirée RWSB</v>
-      </c>
-      <c r="J37" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Factory Club - Soirée RWSB_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Factory Club - Soirée RWSB_x000D_
 &gt; https://vu.fr/fPBPm</v>
       </c>
+      <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="27">
@@ -4797,7 +4703,7 @@
       </c>
       <c r="B38" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Samedi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>88</v>
@@ -4816,17 +4722,14 @@
       </c>
       <c r="H38" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Sam. 🪩 La MAS</v>
+        <v>Jjj. 🪩 La MAS</v>
       </c>
       <c r="I38" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. Connexion Swing - La MAS WCS</v>
-      </c>
-      <c r="J38" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Sam. Connexion Swing - La MAS WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Connexion Swing - La MAS WCS_x000D_
 &gt; https://vu.fr/hjgol</v>
       </c>
+      <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="27">
@@ -4834,7 +4737,7 @@
       </c>
       <c r="B39" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>88</v>
@@ -4853,17 +4756,14 @@
       </c>
       <c r="H39" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 🪩 Happy Sunday</v>
+        <v>Jjj. 🪩 Happy Sunday</v>
       </c>
       <c r="I39" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. La Station - Happy Sunday</v>
-      </c>
-      <c r="J39" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Dim. La Station - Happy Sunday_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. La Station - Happy Sunday_x000D_
 &gt; http://station-danse.fr/</v>
       </c>
+      <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="27">
@@ -4871,7 +4771,7 @@
       </c>
       <c r="B40" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>88</v>
@@ -4890,17 +4790,14 @@
       </c>
       <c r="H40" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 🪩 Sunday WCS</v>
+        <v>Jjj. 🪩 Sunday WCS</v>
       </c>
       <c r="I40" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. TDS - Sunday WCS</v>
-      </c>
-      <c r="J40" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Dim. TDS - Sunday WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Sunday WCS_x000D_
 &gt; https://vu.fr/jspOu</v>
       </c>
+      <c r="J40" s="2"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="27">
@@ -4908,7 +4805,7 @@
       </c>
       <c r="B41" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Mardi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>88</v>
@@ -4927,17 +4824,14 @@
       </c>
       <c r="H41" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Mar. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I41" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mar. TDS - After Mardi</v>
-      </c>
-      <c r="J41" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Mar. TDS - After Mardi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Mardi_x000D_
 &gt; https://vu.fr/GRoSz</v>
       </c>
+      <c r="J41" s="2"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="27">
@@ -4945,7 +4839,7 @@
       </c>
       <c r="B42" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Mercredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>88</v>
@@ -4964,17 +4858,14 @@
       </c>
       <c r="H42" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Mer. 🪩 Happy 1er Mai</v>
+        <v>Jjj. 🪩 Happy 1er Mai</v>
       </c>
       <c r="I42" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mer. La Station - Happy 1er Mai</v>
-      </c>
-      <c r="J42" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Mer. La Station - Happy 1er Mai_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. La Station - Happy 1er Mai_x000D_
 &gt; http://station-danse.fr/</v>
       </c>
+      <c r="J42" s="2"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="27">
@@ -5003,14 +4894,11 @@
         <v>Jeu. 🪩 After TDS</v>
       </c>
       <c r="I43" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Jeu. TDS - After Jeudi</v>
-      </c>
-      <c r="J43" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v>Jeu. TDS - After Jeudi_x000D_
 &gt; https://vu.fr/zTbeO</v>
       </c>
+      <c r="J43" s="2"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="27">
@@ -5018,7 +4906,7 @@
       </c>
       <c r="B44" s="1" t="str">
         <f t="shared" ref="B44:B53" si="2">PROPER(TEXT(A44,"jjjj"))</f>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>88</v>
@@ -5037,17 +4925,14 @@
       </c>
       <c r="H44" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Soirée Factory Club</v>
+        <v>Jjj. 🪩 Soirée Factory Club</v>
       </c>
       <c r="I44" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Factory Club - Soirée RWSB</v>
-      </c>
-      <c r="J44" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Factory Club - Soirée RWSB_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Factory Club - Soirée RWSB_x000D_
 &gt; https://vu.fr/YjdX</v>
       </c>
+      <c r="J44" s="2"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="27">
@@ -5055,7 +4940,7 @@
       </c>
       <c r="B45" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>88</v>
@@ -5072,17 +4957,14 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Level Up Your WCS</v>
+        <v>Jjj. 🪩 Level Up Your WCS</v>
       </c>
       <c r="I45" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Studio Diabolo - Level Up Your WCS</v>
-      </c>
-      <c r="J45" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v xml:space="preserve">Ven. Studio Diabolo - Level Up Your WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v xml:space="preserve">Jjj. Studio Diabolo - Level Up Your WCS_x000D_
 &gt; </v>
       </c>
+      <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="27">
@@ -5090,7 +4972,7 @@
       </c>
       <c r="B46" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Samedi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>120</v>
@@ -5109,17 +4991,14 @@
       </c>
       <c r="H46" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Sam. 📚 Stage Solo Swing TDS</v>
+        <v>Jjj. 📚 Stage Solo Swing TDS</v>
       </c>
       <c r="I46" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. TDS - Stage Solo Swing</v>
-      </c>
-      <c r="J46" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Sam. TDS - Stage Solo Swing_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Stage Solo Swing_x000D_
 &gt; https://vu.fr/YYZsE</v>
       </c>
+      <c r="J46" s="2"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="27">
@@ -5127,7 +5006,7 @@
       </c>
       <c r="B47" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Samedi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>88</v>
@@ -5146,17 +5025,14 @@
       </c>
       <c r="H47" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Sam. 🪩 Soirée TDS</v>
+        <v>Jjj. 🪩 Soirée TDS</v>
       </c>
       <c r="I47" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. TDS - Soirée</v>
-      </c>
-      <c r="J47" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Sam. TDS - Soirée_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Soirée_x000D_
 &gt; https://vu.fr/dLWKf</v>
       </c>
+      <c r="J47" s="2"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="27">
@@ -5164,7 +5040,7 @@
       </c>
       <c r="B48" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>88</v>
@@ -5183,17 +5059,14 @@
       </c>
       <c r="H48" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 🪩 Dimanche WCS</v>
+        <v>Jjj. 🪩 Dimanche WCS</v>
       </c>
       <c r="I48" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. DK'Danse - Dimanche WCS</v>
-      </c>
-      <c r="J48" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Dim. DK'Danse - Dimanche WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. DK'Danse - Dimanche WCS_x000D_
 &gt; https://vu.fr/mNnTC</v>
       </c>
+      <c r="J48" s="2"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="27">
@@ -5201,7 +5074,7 @@
       </c>
       <c r="B49" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>120</v>
@@ -5220,17 +5093,14 @@
       </c>
       <c r="H49" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 📚 Stage TDS</v>
+        <v>Jjj. 📚 Stage TDS</v>
       </c>
       <c r="I49" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. TDS - Stage</v>
-      </c>
-      <c r="J49" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Dim. TDS - Stage_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Stage_x000D_
 &gt; https://vu.fr/MbNjC</v>
       </c>
+      <c r="J49" s="2"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="27">
@@ -5238,7 +5108,7 @@
       </c>
       <c r="B50" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Mardi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>88</v>
@@ -5257,17 +5127,14 @@
       </c>
       <c r="H50" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Mar. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I50" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mar. TDS - After Mardi</v>
-      </c>
-      <c r="J50" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Mar. TDS - After Mardi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Mardi_x000D_
 &gt; https://vu.fr/SJpsc</v>
       </c>
+      <c r="J50" s="2"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="27">
@@ -5275,7 +5142,7 @@
       </c>
       <c r="B51" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Mercredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>88</v>
@@ -5292,17 +5159,14 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Mer. 🪩 WCS Jussieu</v>
+        <v>Jjj. 🪩 WCS Jussieu</v>
       </c>
       <c r="I51" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mer. IMA - WCS Jussieu</v>
-      </c>
-      <c r="J51" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v xml:space="preserve">Mer. IMA - WCS Jussieu_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v xml:space="preserve">Jjj. IMA - WCS Jussieu_x000D_
 &gt; </v>
       </c>
+      <c r="J51" s="2"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="27">
@@ -5310,7 +5174,7 @@
       </c>
       <c r="B52" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Mercredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>73</v>
@@ -5332,14 +5196,11 @@
         <v>WE 🎟️ French Open WCS</v>
       </c>
       <c r="I52" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mer. Event - French Open WCS</v>
-      </c>
-      <c r="J52" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Mer. Event - French Open WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>WE. Event - French Open WCS_x000D_
 &gt; https://www.fowcs.com/</v>
       </c>
+      <c r="J52" s="2"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="27">
@@ -5347,7 +5208,7 @@
       </c>
       <c r="B53" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>88</v>
@@ -5366,17 +5227,14 @@
       </c>
       <c r="H53" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Soirée Factory Club</v>
+        <v>Jjj. 🪩 Soirée Factory Club</v>
       </c>
       <c r="I53" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Factory Club - Soirée RWSB</v>
-      </c>
-      <c r="J53" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Factory Club - Soirée RWSB_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Factory Club - Soirée RWSB_x000D_
 &gt; https://vu.fr/BLjpZ</v>
       </c>
+      <c r="J53" s="2"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="27">
@@ -5405,14 +5263,11 @@
         <v>Dim. 🪩 Happy Sunday</v>
       </c>
       <c r="I54" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. La Station - Happy Sunday</v>
-      </c>
-      <c r="J54" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v>Dim. La Station - Happy Sunday_x000D_
 &gt; http://station-danse.fr/</v>
       </c>
+      <c r="J54" s="2"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="27">
@@ -5420,7 +5275,7 @@
       </c>
       <c r="B55" s="1" t="str">
         <f t="shared" ref="B55:B88" si="3">PROPER(TEXT(A55,"jjjj"))</f>
-        <v>Mardi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>88</v>
@@ -5439,17 +5294,14 @@
       </c>
       <c r="H55" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Mar. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I55" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mar. TDS - After Mardi</v>
-      </c>
-      <c r="J55" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Mar. TDS - After Mardi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Mardi_x000D_
 &gt; https://vu.fr/jvDwd</v>
       </c>
+      <c r="J55" s="2"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="27">
@@ -5457,7 +5309,7 @@
       </c>
       <c r="B56" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Jeudi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>88</v>
@@ -5476,17 +5328,14 @@
       </c>
       <c r="H56" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Jeu. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I56" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Jeu. TDS - After Jeudi</v>
-      </c>
-      <c r="J56" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Jeu. TDS - After Jeudi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Jeudi_x000D_
 &gt; https://vu.fr/WinLA</v>
       </c>
+      <c r="J56" s="2"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="27">
@@ -5494,7 +5343,7 @@
       </c>
       <c r="B57" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>88</v>
@@ -5513,17 +5362,14 @@
       </c>
       <c r="H57" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Factory Club</v>
+        <v>Jjj. 🪩 Factory Club</v>
       </c>
       <c r="I57" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Factory Club - Soirée RWSB</v>
-      </c>
-      <c r="J57" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Factory Club - Soirée RWSB_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Factory Club - Soirée RWSB_x000D_
 &gt; https://vu.fr/fPBPm</v>
       </c>
+      <c r="J57" s="2"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="27">
@@ -5531,7 +5377,7 @@
       </c>
       <c r="B58" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>88</v>
@@ -5550,17 +5396,14 @@
       </c>
       <c r="H58" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Olympiades</v>
+        <v>Jjj. 🪩 Olympiades</v>
       </c>
       <c r="I58" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Sens. Danse - Olympiades</v>
-      </c>
-      <c r="J58" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Sens. Danse - Olympiades_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Sens. Danse - Olympiades_x000D_
 &gt; https://vu.fr/LnCPJ</v>
       </c>
+      <c r="J58" s="2"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="27">
@@ -5568,7 +5411,7 @@
       </c>
       <c r="B59" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>73</v>
@@ -5588,14 +5431,11 @@
         <v>WE 🎟️ West Duck Swing</v>
       </c>
       <c r="I59" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven.  - West Duck Swing</v>
-      </c>
-      <c r="J59" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven.  - West Duck Swing_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>WE.  - West Duck Swing_x000D_
 &gt; https://vu.fr/rVijM</v>
       </c>
+      <c r="J59" s="2"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="27">
@@ -5603,7 +5443,7 @@
       </c>
       <c r="B60" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>73</v>
@@ -5623,14 +5463,11 @@
         <v>WE 🎟️ Med In Swing</v>
       </c>
       <c r="I60" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven.  - Med In Swing</v>
-      </c>
-      <c r="J60" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven.  - Med In Swing_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>WE.  - Med In Swing_x000D_
 &gt; https://vu.fr/moDzi</v>
       </c>
+      <c r="J60" s="2"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="27">
@@ -5638,7 +5475,7 @@
       </c>
       <c r="B61" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>73</v>
@@ -5658,14 +5495,11 @@
         <v>WE 🎟️ Bretzel Swing</v>
       </c>
       <c r="I61" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven.  - Bretzel Swing</v>
-      </c>
-      <c r="J61" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven.  - Bretzel Swing_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>WE.  - Bretzel Swing_x000D_
 &gt; https://vu.fr/NmtYG</v>
       </c>
+      <c r="J61" s="2"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="27">
@@ -5673,7 +5507,7 @@
       </c>
       <c r="B62" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Samedi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>88</v>
@@ -5692,17 +5526,14 @@
       </c>
       <c r="H62" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Sam. 🪩 La MAS</v>
+        <v>Jjj. 🪩 La MAS</v>
       </c>
       <c r="I62" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. Cnx. Swing - La MAS WCS</v>
-      </c>
-      <c r="J62" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Sam. Cnx. Swing - La MAS WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Cnx. Swing - La MAS WCS_x000D_
 &gt; https://vu.fr/LuHTA</v>
       </c>
+      <c r="J62" s="2"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="27">
@@ -5710,7 +5541,7 @@
       </c>
       <c r="B63" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Samedi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>88</v>
@@ -5729,17 +5560,14 @@
       </c>
       <c r="H63" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Sam. 🪩 Mensuelle SDC</v>
+        <v>Jjj. 🪩 Mensuelle SDC</v>
       </c>
       <c r="I63" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. SDC - Mensuelle SDC</v>
-      </c>
-      <c r="J63" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Sam. SDC - Mensuelle SDC_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. SDC - Mensuelle SDC_x000D_
 &gt; https://vu.fr/oTjUx</v>
       </c>
+      <c r="J63" s="2"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="27">
@@ -5747,7 +5575,7 @@
       </c>
       <c r="B64" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>88</v>
@@ -5766,17 +5594,14 @@
       </c>
       <c r="H64" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 🪩 Happy Sunday</v>
+        <v>Jjj. 🪩 Happy Sunday</v>
       </c>
       <c r="I64" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. Station - Happy Sunday</v>
-      </c>
-      <c r="J64" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Dim. Station - Happy Sunday_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Station - Happy Sunday_x000D_
 &gt; http://station-danse.fr/</v>
       </c>
+      <c r="J64" s="2"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="27">
@@ -5784,7 +5609,7 @@
       </c>
       <c r="B65" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Lundi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>88</v>
@@ -5803,17 +5628,14 @@
       </c>
       <c r="H65" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Lun. 🪩 Monday TDS</v>
+        <v>Jjj. 🪩 Monday TDS</v>
       </c>
       <c r="I65" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Lun. TDS - Monday WCS</v>
-      </c>
-      <c r="J65" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Lun. TDS - Monday WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Monday WCS_x000D_
 &gt; https://vu.fr/QvkoY</v>
       </c>
+      <c r="J65" s="2"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="27">
@@ -5821,7 +5643,7 @@
       </c>
       <c r="B66" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Mardi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>88</v>
@@ -5840,17 +5662,14 @@
       </c>
       <c r="H66" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Mar. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I66" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mar. TDS - After Mardi</v>
-      </c>
-      <c r="J66" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Mar. TDS - After Mardi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Mardi_x000D_
 &gt; https://vu.fr/oqmtX</v>
       </c>
+      <c r="J66" s="2"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="27">
@@ -5858,7 +5677,7 @@
       </c>
       <c r="B67" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Jeudi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>88</v>
@@ -5877,17 +5696,14 @@
       </c>
       <c r="H67" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Jeu. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I67" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Jeu. TDS - After Jeudi</v>
-      </c>
-      <c r="J67" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Jeu. TDS - After Jeudi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Jeudi_x000D_
 &gt; https://vu.fr/StuOw</v>
       </c>
+      <c r="J67" s="2"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="27">
@@ -5895,7 +5711,7 @@
       </c>
       <c r="B68" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>88</v>
@@ -5914,17 +5730,14 @@
       </c>
       <c r="H68" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Factory Club</v>
+        <v>Jjj. 🪩 Factory Club</v>
       </c>
       <c r="I68" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Factory Club - Soirée RWSB</v>
-      </c>
-      <c r="J68" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Factory Club - Soirée RWSB_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Factory Club - Soirée RWSB_x000D_
 &gt; https://vu.fr/DUQDs</v>
       </c>
+      <c r="J68" s="2"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="27">
@@ -5932,7 +5745,7 @@
       </c>
       <c r="B69" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Samedi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>88</v>
@@ -5951,17 +5764,14 @@
       </c>
       <c r="H69" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Sam. 🪩 La MAS</v>
+        <v>Jjj. 🪩 La MAS</v>
       </c>
       <c r="I69" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. Cnx. Swing - La MAS WCS</v>
-      </c>
-      <c r="J69" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Sam. Cnx. Swing - La MAS WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Cnx. Swing - La MAS WCS_x000D_
 &gt; https://vu.fr/mkyJC</v>
       </c>
+      <c r="J69" s="2"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="27">
@@ -5969,7 +5779,7 @@
       </c>
       <c r="B70" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Samedi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>88</v>
@@ -5988,17 +5798,14 @@
       </c>
       <c r="H70" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Sam. 🪩 Soirée Dansity</v>
+        <v>Jjj. 🪩 Soirée Dansity</v>
       </c>
       <c r="I70" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. Dansity - Stage &amp; Soirée WCS</v>
-      </c>
-      <c r="J70" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Sam. Dansity - Stage &amp; Soirée WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Dansity - Stage &amp; Soirée WCS_x000D_
 &gt; https://vu.fr/qXNT</v>
       </c>
+      <c r="J70" s="2"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="27">
@@ -6006,7 +5813,7 @@
       </c>
       <c r="B71" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>88</v>
@@ -6025,17 +5832,14 @@
       </c>
       <c r="H71" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 🪩 Happy Sunday</v>
+        <v>Jjj. 🪩 Happy Sunday</v>
       </c>
       <c r="I71" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. Station - Happy Sunday</v>
-      </c>
-      <c r="J71" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Dim. Station - Happy Sunday_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Station - Happy Sunday_x000D_
 &gt; https://vu.fr/FpHCR</v>
       </c>
+      <c r="J71" s="2"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="27">
@@ -6043,7 +5847,7 @@
       </c>
       <c r="B72" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>88</v>
@@ -6062,17 +5866,14 @@
       </c>
       <c r="H72" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 🪩 Sunday WCS</v>
+        <v>Jjj. 🪩 Sunday WCS</v>
       </c>
       <c r="I72" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. TDS - Sunday WCS</v>
-      </c>
-      <c r="J72" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Dim. TDS - Sunday WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Sunday WCS_x000D_
 &gt; https://vu.fr/VlGyX</v>
       </c>
+      <c r="J72" s="2"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="27">
@@ -6080,7 +5881,7 @@
       </c>
       <c r="B73" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>70</v>
@@ -6099,17 +5900,14 @@
       </c>
       <c r="H73" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 🔍 Evaluations Niveau</v>
+        <v>Jjj. 🔍 Evaluations Niveau</v>
       </c>
       <c r="I73" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. TDS - Evaluations Niveau</v>
-      </c>
-      <c r="J73" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Dim. TDS - Evaluations Niveau_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Evaluations Niveau_x000D_
 &gt; https://vu.fr/PYzKe</v>
       </c>
+      <c r="J73" s="2"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="27">
@@ -6117,7 +5915,7 @@
       </c>
       <c r="B74" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Mardi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>88</v>
@@ -6136,17 +5934,14 @@
       </c>
       <c r="H74" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Mar. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I74" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mar. TDS - After Mardi</v>
-      </c>
-      <c r="J74" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Mar. TDS - After Mardi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Mardi_x000D_
 &gt; https://vu.fr/mWwGn</v>
       </c>
+      <c r="J74" s="2"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="27">
@@ -6154,7 +5949,7 @@
       </c>
       <c r="B75" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Jeudi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>88</v>
@@ -6173,17 +5968,14 @@
       </c>
       <c r="H75" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Jeu. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I75" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Jeu. TDS - After Jeudi</v>
-      </c>
-      <c r="J75" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Jeu. TDS - After Jeudi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Jeudi_x000D_
 &gt; https://vu.fr/uPbfe</v>
       </c>
+      <c r="J75" s="2"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="27">
@@ -6191,7 +5983,7 @@
       </c>
       <c r="B76" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>88</v>
@@ -6210,17 +6002,14 @@
       </c>
       <c r="H76" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Factory Club</v>
+        <v>Jjj. 🪩 Factory Club</v>
       </c>
       <c r="I76" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Factory Club - Soirée RWSB</v>
-      </c>
-      <c r="J76" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Factory Club - Soirée RWSB_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Factory Club - Soirée RWSB_x000D_
 &gt; https://vu.fr/DUQDs</v>
       </c>
+      <c r="J76" s="2"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="27">
@@ -6228,7 +6017,7 @@
       </c>
       <c r="B77" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>88</v>
@@ -6247,17 +6036,14 @@
       </c>
       <c r="H77" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 West In Palaiseau</v>
+        <v>Jjj. 🪩 West In Palaiseau</v>
       </c>
       <c r="I77" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Belle Fee Danse - West In Palaiseau</v>
-      </c>
-      <c r="J77" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Belle Fee Danse - West In Palaiseau_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Belle Fee Danse - West In Palaiseau_x000D_
 &gt; https://vu.fr/gKRrP</v>
       </c>
+      <c r="J77" s="2"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="27">
@@ -6265,7 +6051,7 @@
       </c>
       <c r="B78" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>73</v>
@@ -6287,14 +6073,11 @@
         <v>WE 🎟️ West In Honfleur</v>
       </c>
       <c r="I78" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. TDS - West In Honfleur</v>
-      </c>
-      <c r="J78" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. TDS - West In Honfleur_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>WE. TDS - West In Honfleur_x000D_
 &gt; https://vu.fr/maYvf</v>
       </c>
+      <c r="J78" s="2"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="27">
@@ -6302,7 +6085,7 @@
       </c>
       <c r="B79" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Samedi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>88</v>
@@ -6321,17 +6104,14 @@
       </c>
       <c r="H79" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Sam. 🪩 La Boum WCS</v>
+        <v>Jjj. 🪩 La Boum WCS</v>
       </c>
       <c r="I79" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. DK'Danse - La Boum WCS</v>
-      </c>
-      <c r="J79" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Sam. DK'Danse - La Boum WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. DK'Danse - La Boum WCS_x000D_
 &gt; https://vu.fr/dMvyT</v>
       </c>
+      <c r="J79" s="2"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="27">
@@ -6339,7 +6119,7 @@
       </c>
       <c r="B80" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>88</v>
@@ -6358,17 +6138,14 @@
       </c>
       <c r="H80" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 🪩 Happy Sunday</v>
+        <v>Jjj. 🪩 Happy Sunday</v>
       </c>
       <c r="I80" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. Station - Happy Sunday</v>
-      </c>
-      <c r="J80" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Dim. Station - Happy Sunday_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Station - Happy Sunday_x000D_
 &gt; http://station-danse.fr/</v>
       </c>
+      <c r="J80" s="2"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="27">
@@ -6376,7 +6153,7 @@
       </c>
       <c r="B81" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Mardi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>88</v>
@@ -6395,17 +6172,14 @@
       </c>
       <c r="H81" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Mar. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I81" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mar. TDS - After Mardi</v>
-      </c>
-      <c r="J81" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Mar. TDS - After Mardi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Mardi_x000D_
 &gt; https://vu.fr/XiSHX</v>
       </c>
+      <c r="J81" s="2"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="27">
@@ -6413,7 +6187,7 @@
       </c>
       <c r="B82" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Jeudi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>88</v>
@@ -6432,17 +6206,14 @@
       </c>
       <c r="H82" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Jeu. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I82" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Jeu. TDS - After Jeudi</v>
-      </c>
-      <c r="J82" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Jeu. TDS - After Jeudi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Jeudi_x000D_
 &gt; https://vu.fr/hIbv</v>
       </c>
+      <c r="J82" s="2"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="27">
@@ -6450,7 +6221,7 @@
       </c>
       <c r="B83" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>88</v>
@@ -6469,17 +6240,14 @@
       </c>
       <c r="H83" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Factory Club</v>
+        <v>Jjj. 🪩 Factory Club</v>
       </c>
       <c r="I83" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Factory Club - Soirée RWSB</v>
-      </c>
-      <c r="J83" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Factory Club - Soirée RWSB_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Factory Club - Soirée RWSB_x000D_
 &gt; https://vu.fr/DUQDs</v>
       </c>
+      <c r="J83" s="2"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="27">
@@ -6487,7 +6255,7 @@
       </c>
       <c r="B84" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>88</v>
@@ -6506,17 +6274,14 @@
       </c>
       <c r="H84" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Soirée TGIF</v>
+        <v>Jjj. 🪩 Soirée TGIF</v>
       </c>
       <c r="I84" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Studio Diabolo - Soirée TGIF</v>
-      </c>
-      <c r="J84" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Studio Diabolo - Soirée TGIF_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Studio Diabolo - Soirée TGIF_x000D_
 &gt; https://vu.fr/VeJAz</v>
       </c>
+      <c r="J84" s="2"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="27">
@@ -6524,7 +6289,7 @@
       </c>
       <c r="B85" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>73</v>
@@ -6546,14 +6311,11 @@
         <v>WE 🎟️ Westy Welsh</v>
       </c>
       <c r="I85" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. XXL Orga - Westy Welsh</v>
-      </c>
-      <c r="J85" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. XXL Orga - Westy Welsh_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>WE. XXL Orga - Westy Welsh_x000D_
 &gt; https://vu.fr/wJIBI</v>
       </c>
+      <c r="J85" s="2"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="27">
@@ -6561,7 +6323,7 @@
       </c>
       <c r="B86" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Samedi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>70</v>
@@ -6580,17 +6342,14 @@
       </c>
       <c r="H86" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Sam. 🔍 Evaluations Niveau</v>
+        <v>Jjj. 🔍 Evaluations Niveau</v>
       </c>
       <c r="I86" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. TDS - Evaluations Niveau</v>
-      </c>
-      <c r="J86" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Sam. TDS - Evaluations Niveau_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Evaluations Niveau_x000D_
 &gt; https://vu.fr/fSRSP</v>
       </c>
+      <c r="J86" s="2"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="27">
@@ -6598,7 +6357,7 @@
       </c>
       <c r="B87" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>88</v>
@@ -6617,17 +6376,14 @@
       </c>
       <c r="H87" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 🪩 Happy Sunday</v>
+        <v>Jjj. 🪩 Happy Sunday</v>
       </c>
       <c r="I87" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. Station - Happy Sunday</v>
-      </c>
-      <c r="J87" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Dim. Station - Happy Sunday_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Station - Happy Sunday_x000D_
 &gt; https://vu.fr/FpHCR</v>
       </c>
+      <c r="J87" s="2"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="27">
@@ -6635,7 +6391,7 @@
       </c>
       <c r="B88" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Mardi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>88</v>
@@ -6654,17 +6410,14 @@
       </c>
       <c r="H88" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Mar. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I88" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mar. TDS - After Mardi</v>
-      </c>
-      <c r="J88" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Mar. TDS - After Mardi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Mardi_x000D_
 &gt; https://vu.fr/efNyv</v>
       </c>
+      <c r="J88" s="2"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="27">
@@ -6693,14 +6446,11 @@
         <v>Jeu. 🪩 After TDS</v>
       </c>
       <c r="I89" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Jeu. TDS - After Jeudi</v>
-      </c>
-      <c r="J89" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v>Jeu. TDS - After Jeudi_x000D_
 &gt; https://vu.fr/ihZVZ</v>
       </c>
+      <c r="J89" s="2"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="27">
@@ -6708,7 +6458,7 @@
       </c>
       <c r="B90" s="1" t="str">
         <f>PROPER(TEXT(A90,"jjjj"))</f>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>88</v>
@@ -6727,17 +6477,14 @@
       </c>
       <c r="H90" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Soirée Factory Club</v>
+        <v>Jjj. 🪩 Soirée Factory Club</v>
       </c>
       <c r="I90" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Factory Club - Soirée RWSB</v>
-      </c>
-      <c r="J90" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Factory Club - Soirée RWSB_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Factory Club - Soirée RWSB_x000D_
 &gt; https://vu.fr/qlrkq</v>
       </c>
+      <c r="J90" s="2"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="27">
@@ -6745,7 +6492,7 @@
       </c>
       <c r="B91" s="1" t="str">
         <f>PROPER(TEXT(A91,"jjjj"))</f>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>88</v>
@@ -6764,17 +6511,14 @@
       </c>
       <c r="H91" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 La MAS</v>
+        <v>Jjj. 🪩 La MAS</v>
       </c>
       <c r="I91" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Connexion Swing - La MAS WCS</v>
-      </c>
-      <c r="J91" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Connexion Swing - La MAS WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Connexion Swing - La MAS WCS_x000D_
 &gt; https://vu.fr/HiqIT</v>
       </c>
+      <c r="J91" s="2"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="27">
@@ -6782,7 +6526,7 @@
       </c>
       <c r="B92" s="1" t="str">
         <f>PROPER(TEXT(A92,"jjjj"))</f>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>88</v>
@@ -6801,17 +6545,14 @@
       </c>
       <c r="H92" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 🪩 Sunday WCS</v>
+        <v>Jjj. 🪩 Sunday WCS</v>
       </c>
       <c r="I92" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. TDS - Sunday WCS</v>
-      </c>
-      <c r="J92" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Dim. TDS - Sunday WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Sunday WCS_x000D_
 &gt; https://vu.fr/PVoVC</v>
       </c>
+      <c r="J92" s="2"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="27">
@@ -6819,7 +6560,7 @@
       </c>
       <c r="B93" s="1" t="str">
         <f>PROPER(TEXT(A93,"jjjj"))</f>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>120</v>
@@ -6838,17 +6579,14 @@
       </c>
       <c r="H93" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 📚 Solo Swing Follower</v>
+        <v>Jjj. 📚 Solo Swing Follower</v>
       </c>
       <c r="I93" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. TDS - Solo Swing Follower</v>
-      </c>
-      <c r="J93" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Dim. TDS - Solo Swing Follower_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Solo Swing Follower_x000D_
 &gt; https://vu.fr/KUymP</v>
       </c>
+      <c r="J93" s="2"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="27">
@@ -6856,7 +6594,7 @@
       </c>
       <c r="B94" s="1" t="str">
         <f t="shared" ref="B94:B100" si="4">PROPER(TEXT(A94,"jjjj"))</f>
-        <v>Mardi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>88</v>
@@ -6875,17 +6613,14 @@
       </c>
       <c r="H94" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Mar. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I94" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mar. TDS - After Mardi</v>
-      </c>
-      <c r="J94" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Mar. TDS - After Mardi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Mardi_x000D_
 &gt; https://www.facebook.com/events/1656360838165130/1656360881498459</v>
       </c>
+      <c r="J94" s="2"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="27">
@@ -6893,7 +6628,7 @@
       </c>
       <c r="B95" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>Jeudi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>88</v>
@@ -6912,17 +6647,14 @@
       </c>
       <c r="H95" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Jeu. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I95" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Jeu. TDS - After Jeudi</v>
-      </c>
-      <c r="J95" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Jeu. TDS - After Jeudi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Jeudi_x000D_
 &gt; https://www.facebook.com/events/258893990347311/258894053680638</v>
       </c>
+      <c r="J95" s="2"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="27">
@@ -6930,7 +6662,7 @@
       </c>
       <c r="B96" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>88</v>
@@ -6949,17 +6681,14 @@
       </c>
       <c r="H96" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Olympiades</v>
+        <v>Jjj. 🪩 Olympiades</v>
       </c>
       <c r="I96" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Sens. Danse - Olympiades</v>
-      </c>
-      <c r="J96" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Sens. Danse - Olympiades_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Sens. Danse - Olympiades_x000D_
 &gt; https://www.facebook.com/events/981319306334689/1162077968258821</v>
       </c>
+      <c r="J96" s="2"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="27">
@@ -6967,7 +6696,7 @@
       </c>
       <c r="B97" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>88</v>
@@ -6986,17 +6715,14 @@
       </c>
       <c r="H97" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Factory Club</v>
+        <v>Jjj. 🪩 Factory Club</v>
       </c>
       <c r="I97" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Factory Club - Soirée RWSB</v>
-      </c>
-      <c r="J97" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Factory Club - Soirée RWSB_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Factory Club - Soirée RWSB_x000D_
 &gt; https://www.facebook.com/events/380127214568938</v>
       </c>
+      <c r="J97" s="2"/>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="27">
@@ -7004,7 +6730,7 @@
       </c>
       <c r="B98" s="1" t="str">
         <f>PROPER(TEXT(A98,"jjjj"))</f>
-        <v>Samedi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>88</v>
@@ -7023,17 +6749,14 @@
       </c>
       <c r="H98" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Sam. 🪩 La MAS</v>
+        <v>Jjj. 🪩 La MAS</v>
       </c>
       <c r="I98" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. Cnx. Swing - La MAS</v>
-      </c>
-      <c r="J98" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Sam. Cnx. Swing - La MAS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Cnx. Swing - La MAS_x000D_
 &gt; https://www.facebook.com/events/367366285957854</v>
       </c>
+      <c r="J98" s="2"/>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="27">
@@ -7041,7 +6764,7 @@
       </c>
       <c r="B99" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>88</v>
@@ -7060,17 +6783,14 @@
       </c>
       <c r="H99" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 🪩 Happy Sunday</v>
+        <v>Jjj. 🪩 Happy Sunday</v>
       </c>
       <c r="I99" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. La Station - Happy Sunday</v>
-      </c>
-      <c r="J99" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Dim. La Station - Happy Sunday_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. La Station - Happy Sunday_x000D_
 &gt; https://www.facebook.com/stationdanse</v>
       </c>
+      <c r="J99" s="2"/>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="27">
@@ -7078,7 +6798,7 @@
       </c>
       <c r="B100" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>120</v>
@@ -7097,17 +6817,14 @@
       </c>
       <c r="H100" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 📚 Sunday is Private TDS</v>
+        <v>Jjj. 📚 Sunday is Private TDS</v>
       </c>
       <c r="I100" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. TDS - Sunday is Private</v>
-      </c>
-      <c r="J100" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Dim. TDS - Sunday is Private_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Sunday is Private_x000D_
 &gt; https://templeduswing.com/wcs-semi-private-juin-2024/</v>
       </c>
+      <c r="J100" s="2"/>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="27">
@@ -7115,7 +6832,7 @@
       </c>
       <c r="B101" s="1" t="str">
         <f t="shared" ref="B101:B121" si="5">PROPER(TEXT(A101,"jjjj"))</f>
-        <v>Mardi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>88</v>
@@ -7134,17 +6851,14 @@
       </c>
       <c r="H101" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Mar. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I101" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mar. TDS - After Mardi</v>
-      </c>
-      <c r="J101" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Mar. TDS - After Mardi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Mardi_x000D_
 &gt; https://vu.fr/ftMXE</v>
       </c>
+      <c r="J101" s="2"/>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="27">
@@ -7152,7 +6866,7 @@
       </c>
       <c r="B102" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Jeudi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>88</v>
@@ -7171,17 +6885,14 @@
       </c>
       <c r="H102" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Jeu. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I102" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Jeu. TDS - After Jeudi</v>
-      </c>
-      <c r="J102" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Jeu. TDS - After Jeudi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Jeudi_x000D_
 &gt; https://vu.fr/SLvaA</v>
       </c>
+      <c r="J102" s="2"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="27">
@@ -7189,7 +6900,7 @@
       </c>
       <c r="B103" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>88</v>
@@ -7208,17 +6919,14 @@
       </c>
       <c r="H103" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Gala TDS</v>
+        <v>Jjj. 🪩 Gala TDS</v>
       </c>
       <c r="I103" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. TDS - Gala TDS</v>
-      </c>
-      <c r="J103" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. TDS - Gala TDS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Gala TDS_x000D_
 &gt; https://vu.fr/FENnE</v>
       </c>
+      <c r="J103" s="2"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="27">
@@ -7226,7 +6934,7 @@
       </c>
       <c r="B104" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>88</v>
@@ -7245,17 +6953,14 @@
       </c>
       <c r="H104" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Factory Club</v>
+        <v>Jjj. 🪩 Factory Club</v>
       </c>
       <c r="I104" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Factory Club - Soirée RWSB</v>
-      </c>
-      <c r="J104" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Factory Club - Soirée RWSB_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Factory Club - Soirée RWSB_x000D_
 &gt; https://vu.fr/jcWHY</v>
       </c>
+      <c r="J104" s="2"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="27">
@@ -7263,7 +6968,7 @@
       </c>
       <c r="B105" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>88</v>
@@ -7282,17 +6987,14 @@
       </c>
       <c r="H105" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 West In Palaiseau</v>
+        <v>Jjj. 🪩 West In Palaiseau</v>
       </c>
       <c r="I105" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Belle Fee Danse - West In Palaiseau</v>
-      </c>
-      <c r="J105" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Belle Fee Danse - West In Palaiseau_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Belle Fee Danse - West In Palaiseau_x000D_
 &gt; https://vu.fr/VtnR</v>
       </c>
+      <c r="J105" s="2"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="27">
@@ -7300,7 +7002,7 @@
       </c>
       <c r="B106" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Samedi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>88</v>
@@ -7319,17 +7021,14 @@
       </c>
       <c r="H106" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Sam. 🪩 La MAS</v>
+        <v>Jjj. 🪩 La MAS</v>
       </c>
       <c r="I106" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. Cnx. Swing - La MAS</v>
-      </c>
-      <c r="J106" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Sam. Cnx. Swing - La MAS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Cnx. Swing - La MAS_x000D_
 &gt; https://vu.fr/hGlFB</v>
       </c>
+      <c r="J106" s="2"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="27">
@@ -7337,7 +7036,7 @@
       </c>
       <c r="B107" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Samedi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>120</v>
@@ -7356,17 +7055,14 @@
       </c>
       <c r="H107" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Sam. 📚 Form. Prof (Testeurs)</v>
+        <v>Jjj. 📚 Form. Prof (Testeurs)</v>
       </c>
       <c r="I107" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. TDS - Form. Prof (Testeurs)</v>
-      </c>
-      <c r="J107" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Sam. TDS - Form. Prof (Testeurs)_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Form. Prof (Testeurs)_x000D_
 &gt; https://vu.fr/aOaQC</v>
       </c>
+      <c r="J107" s="2"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="27">
@@ -7374,7 +7070,7 @@
       </c>
       <c r="B108" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Dimanche</v>
+        <v>Jjjj</v>
       </c>
       <c r="C108" s="6" t="s">
         <v>88</v>
@@ -7393,17 +7089,14 @@
       </c>
       <c r="H108" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Dim. 🪩 Happy Sunday</v>
+        <v>Jjj. 🪩 Happy Sunday</v>
       </c>
       <c r="I108" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. La Station - Happy Sunday</v>
-      </c>
-      <c r="J108" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Dim. La Station - Happy Sunday_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. La Station - Happy Sunday_x000D_
 &gt; https://vu.fr/goFJh</v>
       </c>
+      <c r="J108" s="2"/>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="27">
@@ -7433,14 +7126,11 @@
         <v>Jjj. 🪩 La BOUM WCS</v>
       </c>
       <c r="I109" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Jjj. DK'Danse - Dimanche WCS</v>
-      </c>
-      <c r="J109" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v>Jjj. DK'Danse - Dimanche WCS_x000D_
 &gt; https://vu.fr/gOomf</v>
       </c>
+      <c r="J109" s="2"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="27">
@@ -7448,7 +7138,7 @@
       </c>
       <c r="B110" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>73</v>
@@ -7470,14 +7160,11 @@
         <v>WE 🎟️ Normandie On West</v>
       </c>
       <c r="I110" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. M&amp;S - Normandie On West</v>
-      </c>
-      <c r="J110" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. M&amp;S - Normandie On West_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>WE. M&amp;S - Normandie On West_x000D_
 &gt; https://vu.fr/nyfV</v>
       </c>
+      <c r="J110" s="2"/>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="27">
@@ -7485,7 +7172,7 @@
       </c>
       <c r="B111" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Lundi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>120</v>
@@ -7504,17 +7191,14 @@
       </c>
       <c r="H111" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Lun. 📚 Intensif Deb+</v>
+        <v>Jjj. 📚 Intensif Deb+</v>
       </c>
       <c r="I111" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Lun. TDS - Intensif Debutant+</v>
-      </c>
-      <c r="J111" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Lun. TDS - Intensif Debutant+_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Intensif Debutant+_x000D_
 &gt; https://vu.fr/nytCj</v>
       </c>
+      <c r="J111" s="2"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="27">
@@ -7522,7 +7206,7 @@
       </c>
       <c r="B112" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Mardi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>88</v>
@@ -7541,17 +7225,14 @@
       </c>
       <c r="H112" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Mar. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I112" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mar. TDS - After Mardi</v>
-      </c>
-      <c r="J112" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Mar. TDS - After Mardi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Mardi_x000D_
 &gt; https://vu.fr/oTIOS</v>
       </c>
+      <c r="J112" s="2"/>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="27">
@@ -7559,7 +7240,7 @@
       </c>
       <c r="B113" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Mercredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>120</v>
@@ -7578,17 +7259,14 @@
       </c>
       <c r="H113" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Mer. 📚 Intensif Inter+</v>
+        <v>Jjj. 📚 Intensif Inter+</v>
       </c>
       <c r="I113" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mer. TDS - Intensif Inter+</v>
-      </c>
-      <c r="J113" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Mer. TDS - Intensif Inter+_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Intensif Inter+_x000D_
 &gt; https://vu.fr/DfEDO</v>
       </c>
+      <c r="J113" s="2"/>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="27">
@@ -7596,7 +7274,7 @@
       </c>
       <c r="B114" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Jeudi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>88</v>
@@ -7615,17 +7293,14 @@
       </c>
       <c r="H114" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Jeu. 🪩 After TDS</v>
+        <v>Jjj. 🪩 After TDS</v>
       </c>
       <c r="I114" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Jeu. TDS - After Jeudi</v>
-      </c>
-      <c r="J114" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Jeu. TDS - After Jeudi_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - After Jeudi_x000D_
 &gt; https://vu.fr/ewPMx</v>
       </c>
+      <c r="J114" s="2"/>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="27">
@@ -7633,7 +7308,7 @@
       </c>
       <c r="B115" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Jeudi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>120</v>
@@ -7652,17 +7327,14 @@
       </c>
       <c r="H115" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Jeu. 📚 Solo Swing F.</v>
+        <v>Jjj. 📚 Solo Swing F.</v>
       </c>
       <c r="I115" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Jeu. TDS - Solo Swing Follower</v>
-      </c>
-      <c r="J115" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Jeu. TDS - Solo Swing Follower_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Solo Swing Follower_x000D_
 &gt; https://vu.fr/NArGq</v>
       </c>
+      <c r="J115" s="2"/>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="27">
@@ -7670,7 +7342,7 @@
       </c>
       <c r="B116" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>70</v>
@@ -7689,17 +7361,14 @@
       </c>
       <c r="H116" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🔍 Evals WCS</v>
+        <v>Jjj. 🔍 Evals WCS</v>
       </c>
       <c r="I116" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. TDS - Evaluations WCS</v>
-      </c>
-      <c r="J116" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. TDS - Evaluations WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Evaluations WCS_x000D_
 &gt; https://vu.fr/ISOjY</v>
       </c>
+      <c r="J116" s="2"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="27">
@@ -7707,7 +7376,7 @@
       </c>
       <c r="B117" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>88</v>
@@ -7726,17 +7395,14 @@
       </c>
       <c r="H117" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Mensuelle SDC</v>
+        <v>Jjj. 🪩 Mensuelle SDC</v>
       </c>
       <c r="I117" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. SDC - Mensuelle SDC</v>
-      </c>
-      <c r="J117" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. SDC - Mensuelle SDC_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. SDC - Mensuelle SDC_x000D_
 &gt; https://vu.fr/JysqU</v>
       </c>
+      <c r="J117" s="2"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="27">
@@ -7744,7 +7410,7 @@
       </c>
       <c r="B118" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>88</v>
@@ -7763,17 +7429,14 @@
       </c>
       <c r="H118" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Soirée TDS</v>
+        <v>Jjj. 🪩 Soirée TDS</v>
       </c>
       <c r="I118" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. TDS - Soirée TDS</v>
-      </c>
-      <c r="J118" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. TDS - Soirée TDS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Soirée TDS_x000D_
 &gt; https://vu.fr/vwrcw</v>
       </c>
+      <c r="J118" s="2"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="27">
@@ -7781,7 +7444,7 @@
       </c>
       <c r="B119" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Vendredi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C119" s="23" t="s">
         <v>88</v>
@@ -7800,17 +7463,14 @@
       </c>
       <c r="H119" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Factory Club</v>
+        <v>Jjj. 🪩 Factory Club</v>
       </c>
       <c r="I119" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Factory Club - Soirée RWSB</v>
-      </c>
-      <c r="J119" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Ven. Factory Club - Soirée RWSB_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. Factory Club - Soirée RWSB_x000D_
 &gt; https://vu.fr/jcWHY</v>
       </c>
+      <c r="J119" s="2"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="27">
@@ -7818,7 +7478,7 @@
       </c>
       <c r="B120" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Samedi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C120" s="6" t="s">
         <v>120</v>
@@ -7837,17 +7497,14 @@
       </c>
       <c r="H120" s="2" t="str">
         <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</f>
-        <v>Sam. 📚 Intensif Init.</v>
+        <v>Jjj. 📚 Intensif Init.</v>
       </c>
       <c r="I120" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. TDS - Initiation WCS</v>
-      </c>
-      <c r="J120" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Sam. TDS - Initiation WCS_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>Jjj. TDS - Initiation WCS_x000D_
 &gt; https://vu.fr/Vzgux</v>
       </c>
+      <c r="J120" s="2"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="27">
@@ -7855,7 +7512,7 @@
       </c>
       <c r="B121" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Samedi</v>
+        <v>Jjjj</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>73</v>
@@ -7877,14 +7534,11 @@
         <v>WE 🎟️ WOTP</v>
       </c>
       <c r="I121" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. Event - WOTP</v>
-      </c>
-      <c r="J121" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Sam. Event - WOTP_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>WE. Event - WOTP_x000D_
 &gt; https://vu.fr/yaYLj</v>
       </c>
+      <c r="J121" s="2"/>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="27">
@@ -7914,13 +7568,12 @@
         <v>Lun. 📚 Intensif Deb+</v>
       </c>
       <c r="I122" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Lun. TDS - Intensif Debutant+</v>
-      </c>
-      <c r="J122" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v>Lun. TDS - Intensif Debutant+_x000D_
 &gt; https://vu.fr/shDvA</v>
+      </c>
+      <c r="J122" s="2" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
@@ -7951,13 +7604,12 @@
         <v>Mar. 🪩 After TDS</v>
       </c>
       <c r="I123" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mar. TDS - After Mardi</v>
-      </c>
-      <c r="J123" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v>Mar. TDS - After Mardi_x000D_
 &gt; https://vu.fr/qBIpB</v>
+      </c>
+      <c r="J123" s="2" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
@@ -7988,13 +7640,12 @@
         <v>Mer. 📚 Intensif Inter+</v>
       </c>
       <c r="I124" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Mer. TDS - Intensif Inter+</v>
-      </c>
-      <c r="J124" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v>Mer. TDS - Intensif Inter+_x000D_
 &gt; https://vu.fr/olGDE</v>
+      </c>
+      <c r="J124" s="2" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
@@ -8025,13 +7676,12 @@
         <v>Jeu. 🪩 After TDS</v>
       </c>
       <c r="I125" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Jeu. TDS - After Jeudi</v>
-      </c>
-      <c r="J125" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v>Jeu. TDS - After Jeudi_x000D_
 &gt; https://vu.fr/tKHqr</v>
+      </c>
+      <c r="J125" s="2" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
@@ -8062,13 +7712,12 @@
         <v>Ven. 🪩 Factory Club</v>
       </c>
       <c r="I126" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Ven. Factory Club - Soirée RWSB</v>
-      </c>
-      <c r="J126" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v>Ven. Factory Club - Soirée RWSB_x000D_
 &gt; https://vu.fr/aoJab</v>
+      </c>
+      <c r="J126" s="2" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
@@ -8099,13 +7748,12 @@
         <v>Dim. 🪩 Happy Sunday</v>
       </c>
       <c r="I127" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Dim. La Station - Happy Sunday</v>
-      </c>
-      <c r="J127" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
         <v>Dim. La Station - Happy Sunday_x000D_
 &gt; https://vu.fr/goFJh</v>
+      </c>
+      <c r="J127" s="2" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
@@ -8136,13 +7784,12 @@
         <v>WE 🎟️ WOTP</v>
       </c>
       <c r="I128" s="2" t="str">
-        <f>LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ". " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]]</f>
-        <v>Sam. Cannes - WOTP</v>
-      </c>
-      <c r="J128" s="2" t="str">
-        <f>TBL_FULL[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
-        <v>Sam. Cannes - WOTP_x000D_
+        <f>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</f>
+        <v>WE. Cannes - WOTP_x000D_
 &gt; https://vu.fr/yaYLj</v>
+      </c>
+      <c r="J128" s="2" t="s">
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -8264,8 +7911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC45321-76E6-43B4-8484-6824D3754D5F}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8279,8 +7926,7 @@
     <col min="10" max="10" width="22.5703125" customWidth="1"/>
     <col min="11" max="11" width="32.7109375" customWidth="1"/>
     <col min="12" max="12" width="26" customWidth="1"/>
-    <col min="13" max="13" width="30.42578125" customWidth="1"/>
-    <col min="14" max="15" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="47.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -8321,10 +7967,10 @@
         <v>271</v>
       </c>
       <c r="M1" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
       <c r="N1" t="s">
-        <v>130</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -8364,13 +8010,12 @@
         <v>Lun. 08 - Intensif Deb+</v>
       </c>
       <c r="M2" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]]</f>
-        <v>Lun. TDS - Intensif Debutant+</v>
-      </c>
-      <c r="N2" s="2" t="str">
-        <f>TblLatest[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
         <v>Lun. TDS - Intensif Debutant+_x000D_
 &gt; https://vu.fr/shDvA</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -8410,13 +8055,12 @@
         <v>Mar. 09 - After TDS</v>
       </c>
       <c r="M3" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]]</f>
-        <v>Mar. TDS - After Mardi</v>
-      </c>
-      <c r="N3" s="2" t="str">
-        <f>TblLatest[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
         <v>Mar. TDS - After Mardi_x000D_
 &gt; https://vu.fr/qBIpB</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -8456,13 +8100,12 @@
         <v>Mer. 10 - Intensif Inter+</v>
       </c>
       <c r="M4" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]]</f>
-        <v>Mer. TDS - Intensif Inter+</v>
-      </c>
-      <c r="N4" s="2" t="str">
-        <f>TblLatest[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
         <v>Mer. TDS - Intensif Inter+_x000D_
 &gt; https://vu.fr/olGDE</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -8502,13 +8145,12 @@
         <v>Jeu. 11 - After TDS</v>
       </c>
       <c r="M5" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]]</f>
-        <v>Jeu. TDS - After Jeudi</v>
-      </c>
-      <c r="N5" s="2" t="str">
-        <f>TblLatest[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
         <v>Jeu. TDS - After Jeudi_x000D_
 &gt; https://vu.fr/tKHqr</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -8548,13 +8190,12 @@
         <v>Ven. 12 - Factory Club</v>
       </c>
       <c r="M6" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]]</f>
-        <v>Ven. Factory Club - Soirée RWSB</v>
-      </c>
-      <c r="N6" s="2" t="str">
-        <f>TblLatest[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
         <v>Ven. Factory Club - Soirée RWSB_x000D_
 &gt; https://vu.fr/aoJab</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -8594,13 +8235,12 @@
         <v>Dim. 14 - Station Danse</v>
       </c>
       <c r="M7" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]]</f>
-        <v>Dim. La Station - Happy Sunday</v>
-      </c>
-      <c r="N7" s="2" t="str">
-        <f>TblLatest[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
         <v>Dim. La Station - Happy Sunday_x000D_
 &gt; https://vu.fr/goFJh</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -8640,13 +8280,12 @@
         <v>Du 06 au 13 - WOTP</v>
       </c>
       <c r="M8" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]]</f>
-        <v>WE. Cannes - WOTP</v>
-      </c>
-      <c r="N8" s="2" t="str">
-        <f>TblLatest[[#This Row],[Infos]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
         <v>WE. Cannes - WOTP_x000D_
 &gt; https://vu.fr/yaYLj</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -8672,7 +8311,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added PNG tile support Added ps1 helper to convert SVG to PNG
</commit_message>
<xml_diff>
--- a/WCS.xlsx
+++ b/WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\git\westie-agenda\westie-agenda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59237C78-FAF2-49BE-8F33-E60AD6C1036D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6BC358-EF5E-4868-AA7D-FC6491A17D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="767" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="289">
   <si>
     <t>Faire le Sondage</t>
   </si>
@@ -891,6 +891,27 @@
   </si>
   <si>
     <t>EVT-WOTP2024-Tile.svg</t>
+  </si>
+  <si>
+    <t>TDS-StageEteDeb-Tile.png</t>
+  </si>
+  <si>
+    <t>TDS-Mardi-Ete-Tile.png</t>
+  </si>
+  <si>
+    <t>TDS-StageEteInter-Tile.png</t>
+  </si>
+  <si>
+    <t>TDS-Jeudi-Ete-Tile.png</t>
+  </si>
+  <si>
+    <t>FAC-Vendredi-Tile.png</t>
+  </si>
+  <si>
+    <t>LSD-Dimanche-Generic-Tile.png</t>
+  </si>
+  <si>
+    <t>EVT-WOTP2024-Tile.png</t>
   </si>
 </sst>
 </file>
@@ -1128,20 +1149,6 @@
   </cellStyles>
   <dxfs count="42">
     <dxf>
-      <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1158,6 +1165,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1203,6 +1217,13 @@
       <alignment horizontal="left"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left"/>
     </dxf>
     <dxf>
@@ -1674,51 +1695,51 @@
     <tableColumn id="6" xr3:uid="{7281A423-F84C-4A96-B4AF-F2A866B96E9A}" name="Sondage" dataDxfId="18">
       <calculatedColumnFormula>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{52F64AB4-B550-4EE3-A161-F4F84BAC2A77}" name="Infos + Lien" dataDxfId="2">
+    <tableColumn id="10" xr3:uid="{52F64AB4-B550-4EE3-A161-F4F84BAC2A77}" name="Infos + Lien" dataDxfId="17">
       <calculatedColumnFormula>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C3C24A01-F990-49C0-96AD-9589DEF3C1DF}" name="Image" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{C3C24A01-F990-49C0-96AD-9589DEF3C1DF}" name="Image" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9E08D3BB-8A20-476F-8B56-C00EF44E04B9}" name="TblLatest" displayName="TblLatest" ref="A1:N8" totalsRowShown="0" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9E08D3BB-8A20-476F-8B56-C00EF44E04B9}" name="TblLatest" displayName="TblLatest" ref="A1:N8" totalsRowShown="0" dataDxfId="15">
   <autoFilter ref="A1:N8" xr:uid="{BD7D0BFF-D107-431C-8453-3E1280F0D854}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M6">
     <sortCondition ref="A1:A6"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{5A32B7B5-F113-4E8A-B61F-4A6A3A219F38}" name="Date Début" dataDxfId="16"/>
-    <tableColumn id="13" xr3:uid="{5939C56E-1752-414F-9B1F-26915CA547CB}" name="Heure Début" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{C842EEE1-6786-415B-92F1-90A15F629A93}" name="Date Fin" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{276A4F50-4151-4619-9D28-3B323183A070}" name="Heure Fin" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{7D76EA45-6B9F-47AA-BC4B-333C0A217D3B}" name="Jour" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{5A32B7B5-F113-4E8A-B61F-4A6A3A219F38}" name="Date Début" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{5939C56E-1752-414F-9B1F-26915CA547CB}" name="Heure Début" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{C842EEE1-6786-415B-92F1-90A15F629A93}" name="Date Fin" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{276A4F50-4151-4619-9D28-3B323183A070}" name="Heure Fin" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{7D76EA45-6B9F-47AA-BC4B-333C0A217D3B}" name="Jour" dataDxfId="10">
       <calculatedColumnFormula>VLOOKUP(PROPER(TEXT(A2,"dddd")),TblDays[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F991CC75-7E43-4E27-BAC1-A13A0DDB4EA2}" name="Type" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{116FD67B-CB4E-4768-8852-B3B7D0487065}" name="Lieu / Ecole" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{4ADFCFB0-CAC8-47AB-B266-B6AB9CB80AAA}" name="Nom" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{D62EB0AF-952F-419A-BDDA-B2803683F3C7}" name="Nom Court" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{A105BFB5-86A5-4432-8027-0B0690E84654}" name="URL" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{13903E95-80BF-4327-8073-66A5B7170295}" name="Sondage" dataDxfId="6">
+    <tableColumn id="3" xr3:uid="{F991CC75-7E43-4E27-BAC1-A13A0DDB4EA2}" name="Type" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{116FD67B-CB4E-4768-8852-B3B7D0487065}" name="Lieu / Ecole" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{4ADFCFB0-CAC8-47AB-B266-B6AB9CB80AAA}" name="Nom" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{D62EB0AF-952F-419A-BDDA-B2803683F3C7}" name="Nom Court" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{A105BFB5-86A5-4432-8027-0B0690E84654}" name="URL" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{13903E95-80BF-4327-8073-66A5B7170295}" name="Sondage" dataDxfId="4">
       <calculatedColumnFormula>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{B7FBBB4C-03E9-4318-B4BF-37524775C9CB}" name="Calendrier" dataDxfId="5">
+    <tableColumn id="14" xr3:uid="{B7FBBB4C-03E9-4318-B4BF-37524775C9CB}" name="Calendrier" dataDxfId="3">
       <calculatedColumnFormula>IF(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]], "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9EE3ABE6-B859-41C5-A834-29D644768C27}" name="Infos + Lien" dataDxfId="3">
+    <tableColumn id="10" xr3:uid="{9EE3ABE6-B859-41C5-A834-29D644768C27}" name="Infos + Lien" dataDxfId="2">
       <calculatedColumnFormula>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3CCCE9DB-4FCC-4478-A1DC-9C0D98780478}" name="Image" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{3CCCE9DB-4FCC-4478-A1DC-9C0D98780478}" name="Image" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D74DDD-8432-4192-A172-BF3ECD73FB3B}" name="TblDays" displayName="TblDays" ref="A1:B8" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D74DDD-8432-4192-A172-BF3ECD73FB3B}" name="TblDays" displayName="TblDays" ref="A1:B8" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:B8" xr:uid="{13D74DDD-8432-4192-A172-BF3ECD73FB3B}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{72BE85DD-EFE9-4638-8C61-73698AE82F8A}" name="Day"/>
@@ -7912,7 +7933,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8015,7 +8036,7 @@
 &gt; https://vu.fr/shDvA</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -8060,7 +8081,7 @@
 &gt; https://vu.fr/qBIpB</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -8105,7 +8126,7 @@
 &gt; https://vu.fr/olGDE</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -8150,7 +8171,7 @@
 &gt; https://vu.fr/tKHqr</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -8195,7 +8216,7 @@
 &gt; https://vu.fr/aoJab</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -8240,7 +8261,7 @@
 &gt; https://vu.fr/goFJh</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -8285,7 +8306,7 @@
 &gt; https://vu.fr/yaYLj</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Content - Week 15/07
</commit_message>
<xml_diff>
--- a/WCS.xlsx
+++ b/WCS.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\git\westie-agenda\westie-agenda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6BC358-EF5E-4868-AA7D-FC6491A17D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB888F5-12AA-4F00-8277-0B0B1AC5F9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="767" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="767" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="How To" sheetId="19" r:id="rId1"/>
     <sheet name="Liens" sheetId="18" r:id="rId2"/>
     <sheet name="Evenements" sheetId="2" r:id="rId3"/>
-    <sheet name="Complet" sheetId="17" r:id="rId4"/>
-    <sheet name="Dernier" sheetId="16" r:id="rId5"/>
-    <sheet name="LOV" sheetId="20" r:id="rId6"/>
+    <sheet name="Dernier" sheetId="16" r:id="rId4"/>
+    <sheet name="LOV" sheetId="20" r:id="rId5"/>
+    <sheet name="Complet-Nouveau" sheetId="21" r:id="rId6"/>
+    <sheet name="Complet-Ancien" sheetId="17" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="Events">Evenements!$E$2:$J$7</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="310">
   <si>
     <t>Faire le Sondage</t>
   </si>
@@ -912,12 +913,78 @@
   </si>
   <si>
     <t>EVT-WOTP2024-Tile.png</t>
+  </si>
+  <si>
+    <t>Stages Pré-After</t>
+  </si>
+  <si>
+    <t>19h30</t>
+  </si>
+  <si>
+    <t>21h00</t>
+  </si>
+  <si>
+    <t>00h15</t>
+  </si>
+  <si>
+    <t>20h00</t>
+  </si>
+  <si>
+    <t>22h30</t>
+  </si>
+  <si>
+    <t>22h00</t>
+  </si>
+  <si>
+    <t>01h30</t>
+  </si>
+  <si>
+    <t>20h30</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/1144333326678800</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/981319306334689/1162077971592154/?active_tab=about</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/2232251107106697</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/987495819395915/987496992729131</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/1953903148373027/1953903155039693</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/986486549847532/986486553180865</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/424327910394962/424327930394960</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/8073251446048022/8073251459381354</t>
+  </si>
+  <si>
+    <t>02h00</t>
+  </si>
+  <si>
+    <t>TDS-StagesPreAfter-Tile.png</t>
+  </si>
+  <si>
+    <t>SDS-Vendredi-Juillet-Tile.png</t>
+  </si>
+  <si>
+    <t>SD-LevelUp-0720-Tile.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ am/pm"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1067,7 +1134,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1142,29 +1209,83 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="57">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ am/pm"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ am/pm"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left"/>
     </dxf>
     <dxf>
       <alignment horizontal="left"/>
@@ -1172,10 +1293,6 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1214,6 +1331,45 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left"/>
     </dxf>
     <dxf>
@@ -1651,7 +1807,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C9594648-A2A5-4767-9EA7-494B4761055E}" name="Tableau2" displayName="Tableau2" ref="A1:J36" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C9594648-A2A5-4767-9EA7-494B4761055E}" name="Tableau2" displayName="Tableau2" ref="A1:J36" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="A1:J36" xr:uid="{C9594648-A2A5-4767-9EA7-494B4761055E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:J34">
     <sortCondition ref="E2:E43"/>
@@ -1659,18 +1815,18 @@
     <sortCondition ref="G2:G43"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="7" xr3:uid="{FFE3F0E6-8345-4ECC-9F6F-0CBD92C0284B}" name="Date Début" dataDxfId="36"/>
-    <tableColumn id="10" xr3:uid="{C13A2709-01CA-44DF-BA12-8F35449BC7C1}" name="Heure Début" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{A646D779-7545-4E42-997E-0D8D9C7BAC10}" name="Date Fin" dataDxfId="34"/>
-    <tableColumn id="8" xr3:uid="{181B49B6-63D9-4D73-B890-48335EB6C583}" name="Heure Fin" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{E4253DAB-007D-4FA3-B630-52C05A39F2F8}" name="Type" dataDxfId="32"/>
-    <tableColumn id="1" xr3:uid="{1120406D-2143-49E8-8E49-3F2FC9BA5DD4}" name="Lieu / Ecole" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{BE77BACF-0974-4C2C-A69B-C204DDBAD755}" name="Nom" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{BCB863FE-7AD4-430C-A8EA-D78232079BA5}" name="Nom Court" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{A2092E45-557A-4801-9F1F-2E723E443C88}" name="Sondage" dataDxfId="28">
+    <tableColumn id="7" xr3:uid="{FFE3F0E6-8345-4ECC-9F6F-0CBD92C0284B}" name="Date Début" dataDxfId="51"/>
+    <tableColumn id="10" xr3:uid="{C13A2709-01CA-44DF-BA12-8F35449BC7C1}" name="Heure Début" dataDxfId="50"/>
+    <tableColumn id="9" xr3:uid="{A646D779-7545-4E42-997E-0D8D9C7BAC10}" name="Date Fin" dataDxfId="49"/>
+    <tableColumn id="8" xr3:uid="{181B49B6-63D9-4D73-B890-48335EB6C583}" name="Heure Fin" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{E4253DAB-007D-4FA3-B630-52C05A39F2F8}" name="Type" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{1120406D-2143-49E8-8E49-3F2FC9BA5DD4}" name="Lieu / Ecole" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{BE77BACF-0974-4C2C-A69B-C204DDBAD755}" name="Nom" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{BCB863FE-7AD4-430C-A8EA-D78232079BA5}" name="Nom Court" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{A2092E45-557A-4801-9F1F-2E723E443C88}" name="Sondage" dataDxfId="43">
       <calculatedColumnFormula>IF(Tableau2[[#This Row],[Type]]="Evaluations",PROPER(TEXT(E2,"jjj")),IF(Tableau2[[#This Row],[Type]]="Soirée",PROPER(TEXT(E2,"jjj")),IF(Tableau2[[#This Row],[Type]]="Evenement","WE",IF(Tableau2[[#This Row],[Type]]="Stage",PROPER(TEXT(E2,"jjj")),"")))) &amp;  " " &amp; IF(Tableau2[[#This Row],[Type]]="Evaluations","🔍",IF(Tableau2[[#This Row],[Type]]="Soirée","🪩",IF(Tableau2[[#This Row],[Type]]="Evenement","🎟️",IF(Tableau2[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; Tableau2[[#This Row],[Nom Court]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{9F26F834-45ED-4237-AEC1-486E8EA6EE56}" name="Infos" dataDxfId="27">
+    <tableColumn id="5" xr3:uid="{9F26F834-45ED-4237-AEC1-486E8EA6EE56}" name="Infos" dataDxfId="42">
       <calculatedColumnFormula>Tableau2[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; Tableau2[[#This Row],[Nom]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1679,73 +1835,107 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{C299B888-6182-43CD-96F9-426BE7578FFF}" name="TBL_FULL" displayName="TBL_FULL" ref="A1:J128" totalsRowShown="0" dataDxfId="26">
-  <autoFilter ref="A1:J128" xr:uid="{C299B888-6182-43CD-96F9-426BE7578FFF}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I93">
-    <sortCondition ref="A1:A93"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9E08D3BB-8A20-476F-8B56-C00EF44E04B9}" name="TblLatest" displayName="TblLatest" ref="A1:N9" totalsRowShown="0" dataDxfId="30">
+  <autoFilter ref="A1:N9" xr:uid="{BD7D0BFF-D107-431C-8453-3E1280F0D854}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M8">
+    <sortCondition ref="A1:A8"/>
   </sortState>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{AE280491-5DD3-4B34-B6B4-E467E3533E06}" name="Date" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{14CA9B6A-CE27-4DA4-ADCF-E0087F4A5F80}" name="Jour" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{165FD0F5-71D5-4EE5-8A33-AF2D4A0B6D4B}" name="Type" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{5DF05ED6-BD5F-4BDE-8E1F-24661E38DC89}" name="Lieu / Ecole" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{FDE8242C-9FDB-40BF-BB9C-18AE740DBBDA}" name="Nom" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{327DFD8C-5F0E-4B97-9441-91F494089929}" name="Nom Court" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{01AAA09B-1A39-4C17-862D-E5CB58879CDD}" name="URL" dataDxfId="19" dataCellStyle="Hyperlink"/>
-    <tableColumn id="6" xr3:uid="{7281A423-F84C-4A96-B4AF-F2A866B96E9A}" name="Sondage" dataDxfId="18">
-      <calculatedColumnFormula>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</calculatedColumnFormula>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{5A32B7B5-F113-4E8A-B61F-4A6A3A219F38}" name="Date Début" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{5939C56E-1752-414F-9B1F-26915CA547CB}" name="Heure Début" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{C842EEE1-6786-415B-92F1-90A15F629A93}" name="Date Fin" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{276A4F50-4151-4619-9D28-3B323183A070}" name="Heure Fin" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{7D76EA45-6B9F-47AA-BC4B-333C0A217D3B}" name="Jour" dataDxfId="1">
+      <calculatedColumnFormula>VLOOKUP(PROPER(TEXT(A2,"dddd")),TblDays[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{52F64AB4-B550-4EE3-A161-F4F84BAC2A77}" name="Infos + Lien" dataDxfId="17">
-      <calculatedColumnFormula>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{F991CC75-7E43-4E27-BAC1-A13A0DDB4EA2}" name="Type" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{116FD67B-CB4E-4768-8852-B3B7D0487065}" name="Lieu / Ecole" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{4ADFCFB0-CAC8-47AB-B266-B6AB9CB80AAA}" name="Nom" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{D62EB0AF-952F-419A-BDDA-B2803683F3C7}" name="Nom Court" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{A105BFB5-86A5-4432-8027-0B0690E84654}" name="URL" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{13903E95-80BF-4327-8073-66A5B7170295}" name="Sondage" dataDxfId="8">
+      <calculatedColumnFormula>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C3C24A01-F990-49C0-96AD-9589DEF3C1DF}" name="Image" dataDxfId="16"/>
+    <tableColumn id="14" xr3:uid="{B7FBBB4C-03E9-4318-B4BF-37524775C9CB}" name="Calendrier" dataDxfId="5">
+      <calculatedColumnFormula>IF(AND(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]],OR(AND(TblLatest[[#This Row],[Heure Début]]="", TblLatest[[#This Row],[Heure Fin]]=""),AND(TblLatest[[#This Row],[Date Fin]]=TblLatest[[#This Row],[Date Début]]+1,TblLatest[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{9EE3ABE6-B859-41C5-A834-29D644768C27}" name="Infos + Lien" dataDxfId="7">
+      <calculatedColumnFormula>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{3CCCE9DB-4FCC-4478-A1DC-9C0D98780478}" name="Image" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9E08D3BB-8A20-476F-8B56-C00EF44E04B9}" name="TblLatest" displayName="TblLatest" ref="A1:N8" totalsRowShown="0" dataDxfId="15">
-  <autoFilter ref="A1:N8" xr:uid="{BD7D0BFF-D107-431C-8453-3E1280F0D854}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M6">
-    <sortCondition ref="A1:A6"/>
-  </sortState>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{5A32B7B5-F113-4E8A-B61F-4A6A3A219F38}" name="Date Début" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{5939C56E-1752-414F-9B1F-26915CA547CB}" name="Heure Début" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{C842EEE1-6786-415B-92F1-90A15F629A93}" name="Date Fin" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{276A4F50-4151-4619-9D28-3B323183A070}" name="Heure Fin" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{7D76EA45-6B9F-47AA-BC4B-333C0A217D3B}" name="Jour" dataDxfId="10">
-      <calculatedColumnFormula>VLOOKUP(PROPER(TEXT(A2,"dddd")),TblDays[],2,FALSE)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{F991CC75-7E43-4E27-BAC1-A13A0DDB4EA2}" name="Type" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{116FD67B-CB4E-4768-8852-B3B7D0487065}" name="Lieu / Ecole" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{4ADFCFB0-CAC8-47AB-B266-B6AB9CB80AAA}" name="Nom" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{D62EB0AF-952F-419A-BDDA-B2803683F3C7}" name="Nom Court" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{A105BFB5-86A5-4432-8027-0B0690E84654}" name="URL" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{13903E95-80BF-4327-8073-66A5B7170295}" name="Sondage" dataDxfId="4">
-      <calculatedColumnFormula>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="14" xr3:uid="{B7FBBB4C-03E9-4318-B4BF-37524775C9CB}" name="Calendrier" dataDxfId="3">
-      <calculatedColumnFormula>IF(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]], "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="10" xr3:uid="{9EE3ABE6-B859-41C5-A834-29D644768C27}" name="Infos + Lien" dataDxfId="2">
-      <calculatedColumnFormula>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{3CCCE9DB-4FCC-4478-A1DC-9C0D98780478}" name="Image" dataDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D74DDD-8432-4192-A172-BF3ECD73FB3B}" name="TblDays" displayName="TblDays" ref="A1:B8" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D74DDD-8432-4192-A172-BF3ECD73FB3B}" name="TblDays" displayName="TblDays" ref="A1:B8" totalsRowShown="0" headerRowDxfId="23">
   <autoFilter ref="A1:B8" xr:uid="{13D74DDD-8432-4192-A172-BF3ECD73FB3B}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{72BE85DD-EFE9-4638-8C61-73698AE82F8A}" name="Day"/>
     <tableColumn id="2" xr3:uid="{F686E82F-E4AF-4E58-8848-DB9F8A68803A}" name="Jour"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3B3137DD-6C50-4A10-8003-2F14BBFFA6ED}" name="TblLatest5" displayName="TblLatest5" ref="A1:N8" totalsRowShown="0" dataDxfId="22">
+  <autoFilter ref="A1:N8" xr:uid="{BD7D0BFF-D107-431C-8453-3E1280F0D854}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M6">
+    <sortCondition ref="A1:A6"/>
+  </sortState>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{ED15D875-A019-4F45-9EAB-1416879DA07B}" name="Date Début" dataDxfId="21"/>
+    <tableColumn id="13" xr3:uid="{A5684061-C972-408F-9859-954121D4BD39}" name="Heure Début" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{118BB872-593E-42DD-A274-BC70C22343C4}" name="Date Fin" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{BDD082DE-A3E8-4EE8-AB24-64607528A7AC}" name="Heure Fin" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{ECF34E70-AEB3-49CB-8249-63D24CDDBDAB}" name="Jour" dataDxfId="17">
+      <calculatedColumnFormula>VLOOKUP(PROPER(TEXT(A2,"dddd")),TblDays[],2,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{2FF93F25-A310-4B52-BD28-289E0E2E18DF}" name="Type" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{E642EDA6-3DAD-4B4D-99D8-BD8555297E8C}" name="Lieu / Ecole" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{08FF766A-3678-4F4D-B044-5253A7C2013F}" name="Nom" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{77D9EBC6-907B-4B7B-AD61-53C30EF3C2DD}" name="Nom Court" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{4924B101-A961-4951-8DEA-E0CE587A04D1}" name="URL" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{5D9F8BBD-56EE-4BF3-9CED-DB696FC52CB1}" name="Sondage" dataDxfId="11">
+      <calculatedColumnFormula>IF(TblLatest5[[#This Row],[Type]]="Evaluations",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Soirée",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest5[[#This Row],[Type]]="Stage",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest5[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest5[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest5[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest5[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest5[[#This Row],[Nom Court]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{AB9E6620-C92E-4350-AFCA-BA7C18CD0C86}" name="Calendrier" dataDxfId="6">
+      <calculatedColumnFormula>IF(AND(TblLatest5[[#This Row],[Date Fin]]&gt;TblLatest5[[#This Row],[Date Début]],OR(AND(TblLatest5[[#This Row],[Heure Début]]="", TblLatest5[[#This Row],[Heure Fin]]=""),AND(TblLatest5[[#This Row],[Date Fin]]=TblLatest5[[#This Row],[Date Début]]+1,TblLatest5[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest5[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest5[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest5[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest5[[#This Row],[Nom Court]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{2CD4E64B-4537-4043-A5BD-B4AE385E8743}" name="Infos + Lien" dataDxfId="10">
+      <calculatedColumnFormula>IF(TblLatest5[[#This Row],[Type]]="Evaluations",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Soirée",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest5[[#This Row],[Type]]="Stage",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest5[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest5[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest5[[#This Row],[URL]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{CDFEF383-58C8-4762-A6D2-D83308862293}" name="Image" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{C299B888-6182-43CD-96F9-426BE7578FFF}" name="TBL_FULL" displayName="TBL_FULL" ref="A1:J128" totalsRowShown="0" dataDxfId="41">
+  <autoFilter ref="A1:J128" xr:uid="{C299B888-6182-43CD-96F9-426BE7578FFF}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I93">
+    <sortCondition ref="A1:A93"/>
+  </sortState>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{AE280491-5DD3-4B34-B6B4-E467E3533E06}" name="Date" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{14CA9B6A-CE27-4DA4-ADCF-E0087F4A5F80}" name="Jour" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{165FD0F5-71D5-4EE5-8A33-AF2D4A0B6D4B}" name="Type" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{5DF05ED6-BD5F-4BDE-8E1F-24661E38DC89}" name="Lieu / Ecole" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{FDE8242C-9FDB-40BF-BB9C-18AE740DBBDA}" name="Nom" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{327DFD8C-5F0E-4B97-9441-91F494089929}" name="Nom Court" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{01AAA09B-1A39-4C17-862D-E5CB58879CDD}" name="URL" dataDxfId="34" dataCellStyle="Hyperlink"/>
+    <tableColumn id="6" xr3:uid="{7281A423-F84C-4A96-B4AF-F2A866B96E9A}" name="Sondage" dataDxfId="33">
+      <calculatedColumnFormula>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{52F64AB4-B550-4EE3-A161-F4F84BAC2A77}" name="Infos + Lien" dataDxfId="32">
+      <calculatedColumnFormula>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{C3C24A01-F990-49C0-96AD-9589DEF3C1DF}" name="Image" dataDxfId="31"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2501,8 +2691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53D23E2-73CD-48EF-BF16-8F4C63AFD3E5}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3490,11 +3680,974 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC45321-76E6-43B4-8484-6824D3754D5F}">
+  <dimension ref="A1:N9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="36.42578125" customWidth="1"/>
+    <col min="9" max="9" width="32.28515625" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" customWidth="1"/>
+    <col min="11" max="11" width="32.7109375" customWidth="1"/>
+    <col min="12" max="12" width="26" customWidth="1"/>
+    <col min="13" max="13" width="105.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="47.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="E1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" t="s">
+        <v>271</v>
+      </c>
+      <c r="M1" t="s">
+        <v>130</v>
+      </c>
+      <c r="N1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="34">
+        <v>45488</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2" s="34">
+        <v>45488</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f>VLOOKUP(PROPER(TEXT(A2,"dddd")),TblDays[],2,FALSE)</f>
+        <v>Lundi</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>301</v>
+      </c>
+      <c r="K2" s="2" t="str">
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
+        <v>Lun. 📚 Intensif Deb+</v>
+      </c>
+      <c r="L2" s="2" t="str">
+        <f>IF(AND(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]],OR(AND(TblLatest[[#This Row],[Heure Début]]="", TblLatest[[#This Row],[Heure Fin]]=""),AND(TblLatest[[#This Row],[Date Fin]]=TblLatest[[#This Row],[Date Début]]+1,TblLatest[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</f>
+        <v>Lun. 15 - Intensif Deb+</v>
+      </c>
+      <c r="M2" s="2" t="str">
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
+        <v>Lun. TDS - Intensif Debutant+_x000D_
+&gt; https://www.facebook.com/events/987495819395915/987496992729131</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="34">
+        <v>45489</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>293</v>
+      </c>
+      <c r="C3" s="34">
+        <v>45489</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f>VLOOKUP(PROPER(TEXT(A3,"dddd")),TblDays[],2,FALSE)</f>
+        <v>Mardi</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>302</v>
+      </c>
+      <c r="K3" s="32" t="str">
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
+        <v>Mar. 📚 Stages Pré-After</v>
+      </c>
+      <c r="L3" s="32" t="str">
+        <f>IF(AND(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]],OR(AND(TblLatest[[#This Row],[Heure Début]]="", TblLatest[[#This Row],[Heure Fin]]=""),AND(TblLatest[[#This Row],[Date Fin]]=TblLatest[[#This Row],[Date Début]]+1,TblLatest[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</f>
+        <v>Mar. 16 - Stages Pré-After</v>
+      </c>
+      <c r="M3" s="32" t="str">
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
+        <v>Mar. TDS - Stages Pré-After_x000D_
+&gt; https://www.facebook.com/events/1953903148373027/1953903155039693</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="34">
+        <v>45489</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="C4" s="34">
+        <v>45490</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f>VLOOKUP(PROPER(TEXT(A4,"dddd")),TblDays[],2,FALSE)</f>
+        <v>Mardi</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>303</v>
+      </c>
+      <c r="K4" s="2" t="str">
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
+        <v>Mar. 🪩 After TDS</v>
+      </c>
+      <c r="L4" s="2" t="str">
+        <f>IF(AND(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]],OR(AND(TblLatest[[#This Row],[Heure Début]]="", TblLatest[[#This Row],[Heure Fin]]=""),AND(TblLatest[[#This Row],[Date Fin]]=TblLatest[[#This Row],[Date Début]]+1,TblLatest[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</f>
+        <v>Mar. 16 - After TDS</v>
+      </c>
+      <c r="M4" s="2" t="str">
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
+        <v>Mar. TDS - After Mardi_x000D_
+&gt; https://www.facebook.com/events/986486549847532/986486553180865</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="34">
+        <v>45490</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="C5" s="34">
+        <v>45490</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>294</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <f>VLOOKUP(PROPER(TEXT(A5,"dddd")),TblDays[],2,FALSE)</f>
+        <v>Mercredi</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>304</v>
+      </c>
+      <c r="K5" s="2" t="str">
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
+        <v>Mer. 📚 Intensif Inter+</v>
+      </c>
+      <c r="L5" s="2" t="str">
+        <f>IF(AND(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]],OR(AND(TblLatest[[#This Row],[Heure Début]]="", TblLatest[[#This Row],[Heure Fin]]=""),AND(TblLatest[[#This Row],[Date Fin]]=TblLatest[[#This Row],[Date Début]]+1,TblLatest[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</f>
+        <v>Mer. 17 - Intensif Inter+</v>
+      </c>
+      <c r="M5" s="2" t="str">
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
+        <v>Mer. TDS - Intensif Inter+_x000D_
+&gt; https://www.facebook.com/events/424327910394962/424327930394960</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="34">
+        <v>45491</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="C6" s="34">
+        <v>45492</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <f>VLOOKUP(PROPER(TEXT(A6,"dddd")),TblDays[],2,FALSE)</f>
+        <v>Jeudi</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>305</v>
+      </c>
+      <c r="K6" s="2" t="str">
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
+        <v>Jeu. 🪩 After TDS</v>
+      </c>
+      <c r="L6" s="2" t="str">
+        <f>IF(AND(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]],OR(AND(TblLatest[[#This Row],[Heure Début]]="", TblLatest[[#This Row],[Heure Fin]]=""),AND(TblLatest[[#This Row],[Date Fin]]=TblLatest[[#This Row],[Date Début]]+1,TblLatest[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</f>
+        <v>Jeu. 18 - After TDS</v>
+      </c>
+      <c r="M6" s="2" t="str">
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
+        <v>Jeu. TDS - After Jeudi_x000D_
+&gt; https://www.facebook.com/events/8073251446048022/8073251459381354</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="34">
+        <v>45492</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>297</v>
+      </c>
+      <c r="C7" s="34">
+        <v>45493</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <f>VLOOKUP(PROPER(TEXT(A7,"dddd")),TblDays[],2,FALSE)</f>
+        <v>Vendredi</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H7" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="K7" s="32" t="str">
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
+        <v>Ven. 🪩 Olympiades</v>
+      </c>
+      <c r="L7" s="32" t="str">
+        <f>IF(AND(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]],OR(AND(TblLatest[[#This Row],[Heure Début]]="", TblLatest[[#This Row],[Heure Fin]]=""),AND(TblLatest[[#This Row],[Date Fin]]=TblLatest[[#This Row],[Date Début]]+1,TblLatest[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</f>
+        <v>Ven. 19 - Olympiades</v>
+      </c>
+      <c r="M7" s="32" t="str">
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
+        <v>Ven. Sens. Danse - Olympiades_x000D_
+&gt; https://www.facebook.com/events/981319306334689/1162077971592154/?active_tab=about</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="34">
+        <v>45492</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>293</v>
+      </c>
+      <c r="C8" s="34">
+        <v>45492</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <f>VLOOKUP(PROPER(TEXT(A8,"dddd")),TblDays[],2,FALSE)</f>
+        <v>Vendredi</v>
+      </c>
+      <c r="F8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" t="s">
+        <v>96</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="K8" s="2" t="str">
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
+        <v>Ven. 🪩 Factory Club</v>
+      </c>
+      <c r="L8" s="2" t="str">
+        <f>IF(AND(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]],OR(AND(TblLatest[[#This Row],[Heure Début]]="", TblLatest[[#This Row],[Heure Fin]]=""),AND(TblLatest[[#This Row],[Date Fin]]=TblLatest[[#This Row],[Date Début]]+1,TblLatest[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</f>
+        <v>Ven. 19 - Factory Club</v>
+      </c>
+      <c r="M8" s="2" t="str">
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
+        <v>Ven. Factory Club - Soirée RWSB_x000D_
+&gt; https://www.facebook.com/events/1144333326678800</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="34">
+        <v>45493</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="C9" s="34">
+        <v>45494</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>296</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <f>VLOOKUP(PROPER(TEXT(A9,"dddd")),TblDays[],2,FALSE)</f>
+        <v>Samedi</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="K9" s="2" t="str">
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
+        <v>Sam. 🪩 Level Up Your WCS</v>
+      </c>
+      <c r="L9" s="2" t="str">
+        <f>IF(AND(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]],OR(AND(TblLatest[[#This Row],[Heure Début]]="", TblLatest[[#This Row],[Heure Fin]]=""),AND(TblLatest[[#This Row],[Date Fin]]=TblLatest[[#This Row],[Date Début]]+1,TblLatest[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</f>
+        <v>Sam. 20 - Level Up Your WCS</v>
+      </c>
+      <c r="M9" s="2" t="str">
+        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
+        <v>Sam. Studio Diabolo - Level Up Your WCS_x000D_
+&gt; https://www.facebook.com/events/2232251107106697</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J8" r:id="rId1" xr:uid="{5D73A72C-0C79-40ED-AA24-DAA42D362463}"/>
+    <hyperlink ref="J7" r:id="rId2" xr:uid="{AE43EA1E-1B17-4D9A-B614-BCD988F2CC23}"/>
+    <hyperlink ref="J2" r:id="rId3" xr:uid="{2902DCF7-845F-4874-9C1E-F291B2722CAD}"/>
+    <hyperlink ref="J3" r:id="rId4" xr:uid="{9E09D651-AF9A-49FE-82EC-8BCD8A08316A}"/>
+    <hyperlink ref="J4" r:id="rId5" xr:uid="{E1304A96-A9B1-4A2D-AE26-75A06B104C2E}"/>
+    <hyperlink ref="J5" r:id="rId6" xr:uid="{01821A44-CA7A-4496-B5C4-8C73978B7DB6}"/>
+    <hyperlink ref="J6" r:id="rId7" xr:uid="{BF2C6F75-3743-46FF-B65F-475830B50DB6}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{43EE54E8-8EBF-43F6-B0AF-5F4B63DC208C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <tableParts count="1">
+    <tablePart r:id="rId10"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7403D3FD-DE48-4FE8-8875-9BA61F0FAD4A}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>255</v>
+      </c>
+      <c r="B7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B11DAF3-FEAA-4BCF-9BB9-43BD5D8098FF}">
+  <dimension ref="A1:N8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="36.42578125" customWidth="1"/>
+    <col min="9" max="9" width="32.28515625" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" customWidth="1"/>
+    <col min="11" max="11" width="32.7109375" customWidth="1"/>
+    <col min="12" max="12" width="26" customWidth="1"/>
+    <col min="13" max="14" width="47.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="E1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" t="s">
+        <v>271</v>
+      </c>
+      <c r="M1" t="s">
+        <v>130</v>
+      </c>
+      <c r="N1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>45481</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1">
+        <v>45481</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="str">
+        <f>VLOOKUP(PROPER(TEXT(A2,"dddd")),TblDays[],2,FALSE)</f>
+        <v>Lundi</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>261</v>
+      </c>
+      <c r="K2" s="2" t="str">
+        <f>IF(TblLatest5[[#This Row],[Type]]="Evaluations",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Soirée",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest5[[#This Row],[Type]]="Stage",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest5[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest5[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest5[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest5[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest5[[#This Row],[Nom Court]]</f>
+        <v>Lun. 📚 Intensif Deb+</v>
+      </c>
+      <c r="L2" s="2" t="str">
+        <f>IF(AND(TblLatest5[[#This Row],[Date Fin]]&gt;TblLatest5[[#This Row],[Date Début]],OR(AND(TblLatest5[[#This Row],[Heure Début]]="", TblLatest5[[#This Row],[Heure Fin]]=""),AND(TblLatest5[[#This Row],[Date Fin]]=TblLatest5[[#This Row],[Date Début]]+1,TblLatest5[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest5[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest5[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest5[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest5[[#This Row],[Nom Court]]</f>
+        <v>Lun. 08 - Intensif Deb+</v>
+      </c>
+      <c r="M2" s="2" t="str">
+        <f>IF(TblLatest5[[#This Row],[Type]]="Evaluations",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Soirée",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest5[[#This Row],[Type]]="Stage",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest5[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest5[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest5[[#This Row],[URL]]</f>
+        <v>Lun. TDS - Intensif Debutant+_x000D_
+&gt; https://vu.fr/shDvA</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
+        <v>45482</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21">
+        <v>45482</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="1" t="str">
+        <f>VLOOKUP(PROPER(TEXT(A3,"dddd")),TblDays[],2,FALSE)</f>
+        <v>Mardi</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="K3" s="2" t="str">
+        <f>IF(TblLatest5[[#This Row],[Type]]="Evaluations",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Soirée",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest5[[#This Row],[Type]]="Stage",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest5[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest5[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest5[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest5[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest5[[#This Row],[Nom Court]]</f>
+        <v>Mar. 🪩 After TDS</v>
+      </c>
+      <c r="L3" s="2" t="str">
+        <f>IF(AND(TblLatest5[[#This Row],[Date Fin]]&gt;TblLatest5[[#This Row],[Date Début]],OR(AND(TblLatest5[[#This Row],[Heure Début]]="", TblLatest5[[#This Row],[Heure Fin]]=""),AND(TblLatest5[[#This Row],[Date Fin]]=TblLatest5[[#This Row],[Date Début]]+1,TblLatest5[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest5[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest5[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest5[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest5[[#This Row],[Nom Court]]</f>
+        <v>Mar. 09 - After TDS</v>
+      </c>
+      <c r="M3" s="2" t="str">
+        <f>IF(TblLatest5[[#This Row],[Type]]="Evaluations",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Soirée",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest5[[#This Row],[Type]]="Stage",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest5[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest5[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest5[[#This Row],[URL]]</f>
+        <v>Mar. TDS - After Mardi_x000D_
+&gt; https://vu.fr/qBIpB</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45483</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1">
+        <v>45483</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="str">
+        <f>VLOOKUP(PROPER(TEXT(A4,"dddd")),TblDays[],2,FALSE)</f>
+        <v>Mercredi</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="K4" s="2" t="str">
+        <f>IF(TblLatest5[[#This Row],[Type]]="Evaluations",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Soirée",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest5[[#This Row],[Type]]="Stage",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest5[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest5[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest5[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest5[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest5[[#This Row],[Nom Court]]</f>
+        <v>Mer. 📚 Intensif Inter+</v>
+      </c>
+      <c r="L4" s="2" t="str">
+        <f>IF(AND(TblLatest5[[#This Row],[Date Fin]]&gt;TblLatest5[[#This Row],[Date Début]],OR(AND(TblLatest5[[#This Row],[Heure Début]]="", TblLatest5[[#This Row],[Heure Fin]]=""),AND(TblLatest5[[#This Row],[Date Fin]]=TblLatest5[[#This Row],[Date Début]]+1,TblLatest5[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest5[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest5[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest5[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest5[[#This Row],[Nom Court]]</f>
+        <v>Mer. 10 - Intensif Inter+</v>
+      </c>
+      <c r="M4" s="2" t="str">
+        <f>IF(TblLatest5[[#This Row],[Type]]="Evaluations",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Soirée",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest5[[#This Row],[Type]]="Stage",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest5[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest5[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest5[[#This Row],[URL]]</f>
+        <v>Mer. TDS - Intensif Inter+_x000D_
+&gt; https://vu.fr/olGDE</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <v>45484</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21">
+        <v>45484</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="1" t="str">
+        <f>VLOOKUP(PROPER(TEXT(A5,"dddd")),TblDays[],2,FALSE)</f>
+        <v>Jeudi</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="K5" s="2" t="str">
+        <f>IF(TblLatest5[[#This Row],[Type]]="Evaluations",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Soirée",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest5[[#This Row],[Type]]="Stage",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest5[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest5[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest5[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest5[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest5[[#This Row],[Nom Court]]</f>
+        <v>Jeu. 🪩 After TDS</v>
+      </c>
+      <c r="L5" s="2" t="str">
+        <f>IF(AND(TblLatest5[[#This Row],[Date Fin]]&gt;TblLatest5[[#This Row],[Date Début]],OR(AND(TblLatest5[[#This Row],[Heure Début]]="", TblLatest5[[#This Row],[Heure Fin]]=""),AND(TblLatest5[[#This Row],[Date Fin]]=TblLatest5[[#This Row],[Date Début]]+1,TblLatest5[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest5[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest5[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest5[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest5[[#This Row],[Nom Court]]</f>
+        <v>Jeu. 11 - After TDS</v>
+      </c>
+      <c r="M5" s="2" t="str">
+        <f>IF(TblLatest5[[#This Row],[Type]]="Evaluations",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Soirée",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest5[[#This Row],[Type]]="Stage",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest5[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest5[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest5[[#This Row],[URL]]</f>
+        <v>Jeu. TDS - After Jeudi_x000D_
+&gt; https://vu.fr/tKHqr</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45485</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1">
+        <v>45485</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="str">
+        <f>VLOOKUP(PROPER(TEXT(A6,"dddd")),TblDays[],2,FALSE)</f>
+        <v>Vendredi</v>
+      </c>
+      <c r="F6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J6" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="K6" s="2" t="str">
+        <f>IF(TblLatest5[[#This Row],[Type]]="Evaluations",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Soirée",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest5[[#This Row],[Type]]="Stage",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest5[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest5[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest5[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest5[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest5[[#This Row],[Nom Court]]</f>
+        <v>Ven. 🪩 Factory Club</v>
+      </c>
+      <c r="L6" s="2" t="str">
+        <f>IF(AND(TblLatest5[[#This Row],[Date Fin]]&gt;TblLatest5[[#This Row],[Date Début]],OR(AND(TblLatest5[[#This Row],[Heure Début]]="", TblLatest5[[#This Row],[Heure Fin]]=""),AND(TblLatest5[[#This Row],[Date Fin]]=TblLatest5[[#This Row],[Date Début]]+1,TblLatest5[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest5[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest5[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest5[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest5[[#This Row],[Nom Court]]</f>
+        <v>Ven. 12 - Factory Club</v>
+      </c>
+      <c r="M6" s="2" t="str">
+        <f>IF(TblLatest5[[#This Row],[Type]]="Evaluations",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Soirée",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest5[[#This Row],[Type]]="Stage",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest5[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest5[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest5[[#This Row],[URL]]</f>
+        <v>Ven. Factory Club - Soirée RWSB_x000D_
+&gt; https://vu.fr/aoJab</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45487</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1">
+        <v>45487</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="str">
+        <f>VLOOKUP(PROPER(TEXT(A7,"dddd")),TblDays[],2,FALSE)</f>
+        <v>Dimanche</v>
+      </c>
+      <c r="F7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" t="s">
+        <v>272</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="K7" t="str">
+        <f>IF(TblLatest5[[#This Row],[Type]]="Evaluations",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Soirée",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest5[[#This Row],[Type]]="Stage",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest5[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest5[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest5[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest5[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest5[[#This Row],[Nom Court]]</f>
+        <v>Dim. 🪩 Station Danse</v>
+      </c>
+      <c r="L7" s="2" t="str">
+        <f>IF(AND(TblLatest5[[#This Row],[Date Fin]]&gt;TblLatest5[[#This Row],[Date Début]],OR(AND(TblLatest5[[#This Row],[Heure Début]]="", TblLatest5[[#This Row],[Heure Fin]]=""),AND(TblLatest5[[#This Row],[Date Fin]]=TblLatest5[[#This Row],[Date Début]]+1,TblLatest5[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest5[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest5[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest5[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest5[[#This Row],[Nom Court]]</f>
+        <v>Dim. 14 - Station Danse</v>
+      </c>
+      <c r="M7" s="2" t="str">
+        <f>IF(TblLatest5[[#This Row],[Type]]="Evaluations",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Soirée",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest5[[#This Row],[Type]]="Stage",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest5[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest5[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest5[[#This Row],[URL]]</f>
+        <v>Dim. La Station - Happy Sunday_x000D_
+&gt; https://vu.fr/goFJh</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45479</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1">
+        <v>45486</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="str">
+        <f>VLOOKUP(PROPER(TEXT(A8,"dddd")),TblDays[],2,FALSE)</f>
+        <v>Samedi</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="K8" s="2" t="str">
+        <f>IF(TblLatest5[[#This Row],[Type]]="Evaluations",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Soirée",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest5[[#This Row],[Type]]="Stage",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest5[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest5[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest5[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest5[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest5[[#This Row],[Nom Court]]</f>
+        <v>WE. 🎟️ WOTP</v>
+      </c>
+      <c r="L8" s="2" t="str">
+        <f>IF(AND(TblLatest5[[#This Row],[Date Fin]]&gt;TblLatest5[[#This Row],[Date Début]],OR(AND(TblLatest5[[#This Row],[Heure Début]]="", TblLatest5[[#This Row],[Heure Fin]]=""),AND(TblLatest5[[#This Row],[Date Fin]]=TblLatest5[[#This Row],[Date Début]]+1,TblLatest5[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest5[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest5[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest5[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest5[[#This Row],[Nom Court]]</f>
+        <v>Du 06 au 13 - WOTP</v>
+      </c>
+      <c r="M8" s="2" t="str">
+        <f>IF(TblLatest5[[#This Row],[Type]]="Evaluations",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Soirée",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest5[[#This Row],[Type]]="Stage",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest5[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest5[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest5[[#This Row],[URL]]</f>
+        <v>WE. Cannes - WOTP_x000D_
+&gt; https://vu.fr/yaYLj</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J8" r:id="rId1" xr:uid="{D498D851-34B6-414C-A606-02EB3971D90C}"/>
+    <hyperlink ref="J7" r:id="rId2" xr:uid="{37E6870E-C48E-49B2-A1CE-9CFA79C2070F}"/>
+    <hyperlink ref="J6" r:id="rId3" xr:uid="{1C58F251-D3D1-46AB-8270-FFCBEDFCACDF}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{F17428E6-79CE-44AC-9019-FA066B1E3C70}"/>
+    <hyperlink ref="J4" r:id="rId5" xr:uid="{61895C52-3885-47D5-BC14-E975F9EDD0ED}"/>
+    <hyperlink ref="J3" r:id="rId6" xr:uid="{238F9ECB-B698-4A1D-A378-46268B608423}"/>
+    <hyperlink ref="J2" r:id="rId7" xr:uid="{56EA36F2-317C-4DDF-AC90-AAB5295D40B4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <tableParts count="1">
+    <tablePart r:id="rId9"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB9F931-09B4-4724-BB11-DDCAA6AA5863}">
   <dimension ref="A1:J128"/>
   <sheetViews>
-    <sheetView topLeftCell="C106" workbookViewId="0">
-      <selection activeCell="I136" sqref="I136"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D133" sqref="A133:D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7926,489 +9079,4 @@
     <tablePart r:id="rId106"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC45321-76E6-43B4-8484-6824D3754D5F}">
-  <dimension ref="A1:N8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="36.42578125" customWidth="1"/>
-    <col min="9" max="9" width="32.28515625" customWidth="1"/>
-    <col min="10" max="10" width="22.5703125" customWidth="1"/>
-    <col min="11" max="11" width="32.7109375" customWidth="1"/>
-    <col min="12" max="12" width="26" customWidth="1"/>
-    <col min="13" max="14" width="47.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>267</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>266</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>268</v>
-      </c>
-      <c r="E1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" t="s">
-        <v>271</v>
-      </c>
-      <c r="M1" t="s">
-        <v>130</v>
-      </c>
-      <c r="N1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>45481</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1">
-        <v>45481</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="str">
-        <f>VLOOKUP(PROPER(TEXT(A2,"dddd")),TblDays[],2,FALSE)</f>
-        <v>Lundi</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>261</v>
-      </c>
-      <c r="K2" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
-        <v>Lun. 📚 Intensif Deb+</v>
-      </c>
-      <c r="L2" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]], "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</f>
-        <v>Lun. 08 - Intensif Deb+</v>
-      </c>
-      <c r="M2" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
-        <v>Lun. TDS - Intensif Debutant+_x000D_
-&gt; https://vu.fr/shDvA</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="21">
-        <v>45482</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21">
-        <v>45482</v>
-      </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="1" t="str">
-        <f>VLOOKUP(PROPER(TEXT(A3,"dddd")),TblDays[],2,FALSE)</f>
-        <v>Mardi</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="J3" s="22" t="s">
-        <v>262</v>
-      </c>
-      <c r="K3" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
-        <v>Mar. 🪩 After TDS</v>
-      </c>
-      <c r="L3" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]], "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</f>
-        <v>Mar. 09 - After TDS</v>
-      </c>
-      <c r="M3" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
-        <v>Mar. TDS - After Mardi_x000D_
-&gt; https://vu.fr/qBIpB</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>45483</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1">
-        <v>45483</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="str">
-        <f>VLOOKUP(PROPER(TEXT(A4,"dddd")),TblDays[],2,FALSE)</f>
-        <v>Mercredi</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="J4" s="22" t="s">
-        <v>263</v>
-      </c>
-      <c r="K4" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
-        <v>Mer. 📚 Intensif Inter+</v>
-      </c>
-      <c r="L4" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]], "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</f>
-        <v>Mer. 10 - Intensif Inter+</v>
-      </c>
-      <c r="M4" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
-        <v>Mer. TDS - Intensif Inter+_x000D_
-&gt; https://vu.fr/olGDE</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
-        <v>45484</v>
-      </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21">
-        <v>45484</v>
-      </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="1" t="str">
-        <f>VLOOKUP(PROPER(TEXT(A5,"dddd")),TblDays[],2,FALSE)</f>
-        <v>Jeudi</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="J5" s="22" t="s">
-        <v>264</v>
-      </c>
-      <c r="K5" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
-        <v>Jeu. 🪩 After TDS</v>
-      </c>
-      <c r="L5" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]], "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</f>
-        <v>Jeu. 11 - After TDS</v>
-      </c>
-      <c r="M5" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
-        <v>Jeu. TDS - After Jeudi_x000D_
-&gt; https://vu.fr/tKHqr</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>45485</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1">
-        <v>45485</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="str">
-        <f>VLOOKUP(PROPER(TEXT(A6,"dddd")),TblDays[],2,FALSE)</f>
-        <v>Vendredi</v>
-      </c>
-      <c r="F6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G6" t="s">
-        <v>96</v>
-      </c>
-      <c r="H6" t="s">
-        <v>97</v>
-      </c>
-      <c r="I6" t="s">
-        <v>96</v>
-      </c>
-      <c r="J6" s="24" t="s">
-        <v>265</v>
-      </c>
-      <c r="K6" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
-        <v>Ven. 🪩 Factory Club</v>
-      </c>
-      <c r="L6" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]], "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</f>
-        <v>Ven. 12 - Factory Club</v>
-      </c>
-      <c r="M6" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
-        <v>Ven. Factory Club - Soirée RWSB_x000D_
-&gt; https://vu.fr/aoJab</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>45487</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1">
-        <v>45487</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="str">
-        <f>VLOOKUP(PROPER(TEXT(A7,"dddd")),TblDays[],2,FALSE)</f>
-        <v>Dimanche</v>
-      </c>
-      <c r="F7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G7" t="s">
-        <v>100</v>
-      </c>
-      <c r="H7" t="s">
-        <v>102</v>
-      </c>
-      <c r="I7" t="s">
-        <v>272</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="K7" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
-        <v>Dim. 🪩 Station Danse</v>
-      </c>
-      <c r="L7" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]], "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</f>
-        <v>Dim. 14 - Station Danse</v>
-      </c>
-      <c r="M7" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
-        <v>Dim. La Station - Happy Sunday_x000D_
-&gt; https://vu.fr/goFJh</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>45479</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1">
-        <v>45486</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="str">
-        <f>VLOOKUP(PROPER(TEXT(A8,"dddd")),TblDays[],2,FALSE)</f>
-        <v>Samedi</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="K8" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
-        <v>WE. 🎟️ WOTP</v>
-      </c>
-      <c r="L8" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]], "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</f>
-        <v>Du 06 au 13 - WOTP</v>
-      </c>
-      <c r="M8" s="2" t="str">
-        <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
-        <v>WE. Cannes - WOTP_x000D_
-&gt; https://vu.fr/yaYLj</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="J8" r:id="rId1" xr:uid="{DCC0FF36-A4A9-4976-9864-24A359759802}"/>
-    <hyperlink ref="J7" r:id="rId2" xr:uid="{19B51DDA-5B09-4B25-8575-71130E7AE1DA}"/>
-    <hyperlink ref="J6" r:id="rId3" xr:uid="{4CE286C6-04D4-4882-8BD8-5B55B4F5DDD1}"/>
-    <hyperlink ref="J5" r:id="rId4" xr:uid="{F91A019C-83CE-427F-BD6F-356498900320}"/>
-    <hyperlink ref="J4" r:id="rId5" xr:uid="{EF655DAA-001C-4CC8-9AA4-F97931251DD8}"/>
-    <hyperlink ref="J3" r:id="rId6" xr:uid="{E9DFB5A7-452C-476A-8F1D-489C30847755}"/>
-    <hyperlink ref="J2" r:id="rId7" xr:uid="{C7C44614-8FDD-4399-B5D4-97029B80A3F3}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
-  <tableParts count="1">
-    <tablePart r:id="rId9"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7403D3FD-DE48-4FE8-8875-9BA61F0FAD4A}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>249</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>250</v>
-      </c>
-      <c r="B2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>252</v>
-      </c>
-      <c r="B3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>253</v>
-      </c>
-      <c r="B4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>259</v>
-      </c>
-      <c r="B5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>254</v>
-      </c>
-      <c r="B6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>255</v>
-      </c>
-      <c r="B7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>256</v>
-      </c>
-      <c r="B8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Content - Week 15/07 - Update
</commit_message>
<xml_diff>
--- a/WCS.xlsx
+++ b/WCS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\git\westie-agenda\westie-agenda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\git\westie-agenda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB888F5-12AA-4F00-8277-0B0B1AC5F9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74919462-33ED-47FF-B5DA-172A93114007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="767" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="767" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="How To" sheetId="19" r:id="rId1"/>
@@ -942,30 +942,6 @@
     <t>20h30</t>
   </si>
   <si>
-    <t>https://www.facebook.com/events/1144333326678800</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/events/981319306334689/1162077971592154/?active_tab=about</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/events/2232251107106697</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/events/987495819395915/987496992729131</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/events/1953903148373027/1953903155039693</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/events/986486549847532/986486553180865</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/events/424327910394962/424327930394960</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/events/8073251446048022/8073251459381354</t>
-  </si>
-  <si>
     <t>02h00</t>
   </si>
   <si>
@@ -976,6 +952,30 @@
   </si>
   <si>
     <t>SD-LevelUp-0720-Tile.png</t>
+  </si>
+  <si>
+    <t>https://vu.fr/bARHa</t>
+  </si>
+  <si>
+    <t>https://vu.fr/ndqSl</t>
+  </si>
+  <si>
+    <t>https://vu.fr/PBIgb</t>
+  </si>
+  <si>
+    <t>https://vu.fr/RnOqv</t>
+  </si>
+  <si>
+    <t>https://vu.fr/OvDBA</t>
+  </si>
+  <si>
+    <t>https://vu.fr/qZuKF</t>
+  </si>
+  <si>
+    <t>https://vu.fr/wZdKU</t>
+  </si>
+  <si>
+    <t>https://vu.fr/Ubhqp</t>
   </si>
 </sst>
 </file>
@@ -983,7 +983,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ am/pm"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1134,7 +1134,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1209,16 +1209,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1228,56 +1219,7 @@
   </cellStyles>
   <dxfs count="57">
     <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ am/pm"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ am/pm"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1288,11 +1230,47 @@
       <alignment horizontal="left"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1358,29 +1336,12 @@
       <alignment horizontal="left"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1406,11 +1367,41 @@
       <alignment horizontal="left"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
       <alignment horizontal="left"/>
@@ -1835,41 +1826,41 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9E08D3BB-8A20-476F-8B56-C00EF44E04B9}" name="TblLatest" displayName="TblLatest" ref="A1:N9" totalsRowShown="0" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9E08D3BB-8A20-476F-8B56-C00EF44E04B9}" name="TblLatest" displayName="TblLatest" ref="A1:N9" totalsRowShown="0" dataDxfId="41">
   <autoFilter ref="A1:N9" xr:uid="{BD7D0BFF-D107-431C-8453-3E1280F0D854}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M8">
     <sortCondition ref="A1:A8"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{5A32B7B5-F113-4E8A-B61F-4A6A3A219F38}" name="Date Début" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{5939C56E-1752-414F-9B1F-26915CA547CB}" name="Heure Début" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{C842EEE1-6786-415B-92F1-90A15F629A93}" name="Date Fin" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{276A4F50-4151-4619-9D28-3B323183A070}" name="Heure Fin" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{7D76EA45-6B9F-47AA-BC4B-333C0A217D3B}" name="Jour" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{5A32B7B5-F113-4E8A-B61F-4A6A3A219F38}" name="Date Début" dataDxfId="40"/>
+    <tableColumn id="13" xr3:uid="{5939C56E-1752-414F-9B1F-26915CA547CB}" name="Heure Début" dataDxfId="39"/>
+    <tableColumn id="12" xr3:uid="{C842EEE1-6786-415B-92F1-90A15F629A93}" name="Date Fin" dataDxfId="38"/>
+    <tableColumn id="11" xr3:uid="{276A4F50-4151-4619-9D28-3B323183A070}" name="Heure Fin" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{7D76EA45-6B9F-47AA-BC4B-333C0A217D3B}" name="Jour" dataDxfId="36">
       <calculatedColumnFormula>VLOOKUP(PROPER(TEXT(A2,"dddd")),TblDays[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F991CC75-7E43-4E27-BAC1-A13A0DDB4EA2}" name="Type" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{116FD67B-CB4E-4768-8852-B3B7D0487065}" name="Lieu / Ecole" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{4ADFCFB0-CAC8-47AB-B266-B6AB9CB80AAA}" name="Nom" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{D62EB0AF-952F-419A-BDDA-B2803683F3C7}" name="Nom Court" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{A105BFB5-86A5-4432-8027-0B0690E84654}" name="URL" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{13903E95-80BF-4327-8073-66A5B7170295}" name="Sondage" dataDxfId="8">
+    <tableColumn id="3" xr3:uid="{F991CC75-7E43-4E27-BAC1-A13A0DDB4EA2}" name="Type" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{116FD67B-CB4E-4768-8852-B3B7D0487065}" name="Lieu / Ecole" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{4ADFCFB0-CAC8-47AB-B266-B6AB9CB80AAA}" name="Nom" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{D62EB0AF-952F-419A-BDDA-B2803683F3C7}" name="Nom Court" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{A105BFB5-86A5-4432-8027-0B0690E84654}" name="URL" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{13903E95-80BF-4327-8073-66A5B7170295}" name="Sondage" dataDxfId="30">
       <calculatedColumnFormula>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{B7FBBB4C-03E9-4318-B4BF-37524775C9CB}" name="Calendrier" dataDxfId="5">
+    <tableColumn id="14" xr3:uid="{B7FBBB4C-03E9-4318-B4BF-37524775C9CB}" name="Calendrier" dataDxfId="29">
       <calculatedColumnFormula>IF(AND(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]],OR(AND(TblLatest[[#This Row],[Heure Début]]="", TblLatest[[#This Row],[Heure Fin]]=""),AND(TblLatest[[#This Row],[Date Fin]]=TblLatest[[#This Row],[Date Début]]+1,TblLatest[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9EE3ABE6-B859-41C5-A834-29D644768C27}" name="Infos + Lien" dataDxfId="7">
+    <tableColumn id="10" xr3:uid="{9EE3ABE6-B859-41C5-A834-29D644768C27}" name="Infos + Lien" dataDxfId="28">
       <calculatedColumnFormula>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3CCCE9DB-4FCC-4478-A1DC-9C0D98780478}" name="Image" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{3CCCE9DB-4FCC-4478-A1DC-9C0D98780478}" name="Image" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D74DDD-8432-4192-A172-BF3ECD73FB3B}" name="TblDays" displayName="TblDays" ref="A1:B8" totalsRowShown="0" headerRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D74DDD-8432-4192-A172-BF3ECD73FB3B}" name="TblDays" displayName="TblDays" ref="A1:B8" totalsRowShown="0" headerRowDxfId="26">
   <autoFilter ref="A1:B8" xr:uid="{13D74DDD-8432-4192-A172-BF3ECD73FB3B}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{72BE85DD-EFE9-4638-8C61-73698AE82F8A}" name="Day"/>
@@ -1880,60 +1871,60 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3B3137DD-6C50-4A10-8003-2F14BBFFA6ED}" name="TblLatest5" displayName="TblLatest5" ref="A1:N8" totalsRowShown="0" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3B3137DD-6C50-4A10-8003-2F14BBFFA6ED}" name="TblLatest5" displayName="TblLatest5" ref="A1:N8" totalsRowShown="0" dataDxfId="25">
   <autoFilter ref="A1:N8" xr:uid="{BD7D0BFF-D107-431C-8453-3E1280F0D854}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M6">
     <sortCondition ref="A1:A6"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{ED15D875-A019-4F45-9EAB-1416879DA07B}" name="Date Début" dataDxfId="21"/>
-    <tableColumn id="13" xr3:uid="{A5684061-C972-408F-9859-954121D4BD39}" name="Heure Début" dataDxfId="20"/>
-    <tableColumn id="12" xr3:uid="{118BB872-593E-42DD-A274-BC70C22343C4}" name="Date Fin" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{BDD082DE-A3E8-4EE8-AB24-64607528A7AC}" name="Heure Fin" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{ECF34E70-AEB3-49CB-8249-63D24CDDBDAB}" name="Jour" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{ED15D875-A019-4F45-9EAB-1416879DA07B}" name="Date Début" dataDxfId="24"/>
+    <tableColumn id="13" xr3:uid="{A5684061-C972-408F-9859-954121D4BD39}" name="Heure Début" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{118BB872-593E-42DD-A274-BC70C22343C4}" name="Date Fin" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{BDD082DE-A3E8-4EE8-AB24-64607528A7AC}" name="Heure Fin" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{ECF34E70-AEB3-49CB-8249-63D24CDDBDAB}" name="Jour" dataDxfId="20">
       <calculatedColumnFormula>VLOOKUP(PROPER(TEXT(A2,"dddd")),TblDays[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{2FF93F25-A310-4B52-BD28-289E0E2E18DF}" name="Type" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{E642EDA6-3DAD-4B4D-99D8-BD8555297E8C}" name="Lieu / Ecole" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{08FF766A-3678-4F4D-B044-5253A7C2013F}" name="Nom" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{77D9EBC6-907B-4B7B-AD61-53C30EF3C2DD}" name="Nom Court" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{4924B101-A961-4951-8DEA-E0CE587A04D1}" name="URL" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{5D9F8BBD-56EE-4BF3-9CED-DB696FC52CB1}" name="Sondage" dataDxfId="11">
+    <tableColumn id="3" xr3:uid="{2FF93F25-A310-4B52-BD28-289E0E2E18DF}" name="Type" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{E642EDA6-3DAD-4B4D-99D8-BD8555297E8C}" name="Lieu / Ecole" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{08FF766A-3678-4F4D-B044-5253A7C2013F}" name="Nom" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{77D9EBC6-907B-4B7B-AD61-53C30EF3C2DD}" name="Nom Court" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{4924B101-A961-4951-8DEA-E0CE587A04D1}" name="URL" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{5D9F8BBD-56EE-4BF3-9CED-DB696FC52CB1}" name="Sondage" dataDxfId="14">
       <calculatedColumnFormula>IF(TblLatest5[[#This Row],[Type]]="Evaluations",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Soirée",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest5[[#This Row],[Type]]="Stage",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest5[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest5[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest5[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest5[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest5[[#This Row],[Nom Court]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{AB9E6620-C92E-4350-AFCA-BA7C18CD0C86}" name="Calendrier" dataDxfId="6">
+    <tableColumn id="14" xr3:uid="{AB9E6620-C92E-4350-AFCA-BA7C18CD0C86}" name="Calendrier" dataDxfId="13">
       <calculatedColumnFormula>IF(AND(TblLatest5[[#This Row],[Date Fin]]&gt;TblLatest5[[#This Row],[Date Début]],OR(AND(TblLatest5[[#This Row],[Heure Début]]="", TblLatest5[[#This Row],[Heure Fin]]=""),AND(TblLatest5[[#This Row],[Date Fin]]=TblLatest5[[#This Row],[Date Début]]+1,TblLatest5[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest5[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest5[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest5[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest5[[#This Row],[Nom Court]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{2CD4E64B-4537-4043-A5BD-B4AE385E8743}" name="Infos + Lien" dataDxfId="10">
+    <tableColumn id="10" xr3:uid="{2CD4E64B-4537-4043-A5BD-B4AE385E8743}" name="Infos + Lien" dataDxfId="12">
       <calculatedColumnFormula>IF(TblLatest5[[#This Row],[Type]]="Evaluations",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Soirée",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest5[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest5[[#This Row],[Type]]="Stage",LEFT(TblLatest5[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest5[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest5[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest5[[#This Row],[URL]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{CDFEF383-58C8-4762-A6D2-D83308862293}" name="Image" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{CDFEF383-58C8-4762-A6D2-D83308862293}" name="Image" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{C299B888-6182-43CD-96F9-426BE7578FFF}" name="TBL_FULL" displayName="TBL_FULL" ref="A1:J128" totalsRowShown="0" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{C299B888-6182-43CD-96F9-426BE7578FFF}" name="TBL_FULL" displayName="TBL_FULL" ref="A1:J128" totalsRowShown="0" dataDxfId="10">
   <autoFilter ref="A1:J128" xr:uid="{C299B888-6182-43CD-96F9-426BE7578FFF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I93">
     <sortCondition ref="A1:A93"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{AE280491-5DD3-4B34-B6B4-E467E3533E06}" name="Date" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{14CA9B6A-CE27-4DA4-ADCF-E0087F4A5F80}" name="Jour" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{165FD0F5-71D5-4EE5-8A33-AF2D4A0B6D4B}" name="Type" dataDxfId="38"/>
-    <tableColumn id="8" xr3:uid="{5DF05ED6-BD5F-4BDE-8E1F-24661E38DC89}" name="Lieu / Ecole" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{FDE8242C-9FDB-40BF-BB9C-18AE740DBBDA}" name="Nom" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{327DFD8C-5F0E-4B97-9441-91F494089929}" name="Nom Court" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{01AAA09B-1A39-4C17-862D-E5CB58879CDD}" name="URL" dataDxfId="34" dataCellStyle="Hyperlink"/>
-    <tableColumn id="6" xr3:uid="{7281A423-F84C-4A96-B4AF-F2A866B96E9A}" name="Sondage" dataDxfId="33">
+    <tableColumn id="1" xr3:uid="{AE280491-5DD3-4B34-B6B4-E467E3533E06}" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{14CA9B6A-CE27-4DA4-ADCF-E0087F4A5F80}" name="Jour" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{165FD0F5-71D5-4EE5-8A33-AF2D4A0B6D4B}" name="Type" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{5DF05ED6-BD5F-4BDE-8E1F-24661E38DC89}" name="Lieu / Ecole" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{FDE8242C-9FDB-40BF-BB9C-18AE740DBBDA}" name="Nom" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{327DFD8C-5F0E-4B97-9441-91F494089929}" name="Nom Court" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{01AAA09B-1A39-4C17-862D-E5CB58879CDD}" name="URL" dataDxfId="3" dataCellStyle="Hyperlink"/>
+    <tableColumn id="6" xr3:uid="{7281A423-F84C-4A96-B4AF-F2A866B96E9A}" name="Sondage" dataDxfId="2">
       <calculatedColumnFormula>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TBL_FULL[[#This Row],[Type]]="Evaluations","🔍",IF(TBL_FULL[[#This Row],[Type]]="Soirée","🪩",IF(TBL_FULL[[#This Row],[Type]]="Evenement","🎟️",IF(TBL_FULL[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Nom Court]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{52F64AB4-B550-4EE3-A161-F4F84BAC2A77}" name="Infos + Lien" dataDxfId="32">
+    <tableColumn id="10" xr3:uid="{52F64AB4-B550-4EE3-A161-F4F84BAC2A77}" name="Infos + Lien" dataDxfId="1">
       <calculatedColumnFormula>IF(TBL_FULL[[#This Row],[Type]]="Evaluations",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Soirée",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".",IF(TBL_FULL[[#This Row],[Type]]="Evenement","WE.",IF(TBL_FULL[[#This Row],[Type]]="Stage",LEFT(TBL_FULL[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TBL_FULL[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TBL_FULL[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TBL_FULL[[#This Row],[URL]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C3C24A01-F990-49C0-96AD-9589DEF3C1DF}" name="Image" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{C3C24A01-F990-49C0-96AD-9589DEF3C1DF}" name="Image" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3683,22 +3674,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC45321-76E6-43B4-8484-6824D3754D5F}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="5" max="6" width="13.7109375" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="36.42578125" customWidth="1"/>
     <col min="9" max="9" width="32.28515625" customWidth="1"/>
-    <col min="10" max="10" width="22.5703125" customWidth="1"/>
+    <col min="10" max="10" width="27" customWidth="1"/>
     <col min="11" max="11" width="32.7109375" customWidth="1"/>
-    <col min="12" max="12" width="26" customWidth="1"/>
-    <col min="13" max="13" width="105.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.7109375" customWidth="1"/>
+    <col min="13" max="13" width="63.5703125" customWidth="1"/>
     <col min="14" max="14" width="47.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3747,16 +3737,16 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="34">
+      <c r="A2" s="1">
         <v>45488</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="32" t="s">
         <v>290</v>
       </c>
-      <c r="C2" s="34">
+      <c r="C2" s="1">
         <v>45488</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="32" t="s">
         <v>291</v>
       </c>
       <c r="E2" s="1" t="str">
@@ -3776,7 +3766,7 @@
         <v>231</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K2" s="2" t="str">
         <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
@@ -3789,23 +3779,23 @@
       <c r="M2" s="2" t="str">
         <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
         <v>Lun. TDS - Intensif Debutant+_x000D_
-&gt; https://www.facebook.com/events/987495819395915/987496992729131</v>
+&gt; https://vu.fr/bARHa</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="34">
+      <c r="A3" s="1">
         <v>45489</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="32" t="s">
         <v>293</v>
       </c>
-      <c r="C3" s="34">
+      <c r="C3" s="1">
         <v>45489</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="32" t="s">
         <v>291</v>
       </c>
       <c r="E3" s="1" t="str">
@@ -3825,36 +3815,36 @@
         <v>289</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>302</v>
-      </c>
-      <c r="K3" s="32" t="str">
+        <v>303</v>
+      </c>
+      <c r="K3" s="2" t="str">
         <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
         <v>Mar. 📚 Stages Pré-After</v>
       </c>
-      <c r="L3" s="32" t="str">
+      <c r="L3" s="2" t="str">
         <f>IF(AND(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]],OR(AND(TblLatest[[#This Row],[Heure Début]]="", TblLatest[[#This Row],[Heure Fin]]=""),AND(TblLatest[[#This Row],[Date Fin]]=TblLatest[[#This Row],[Date Début]]+1,TblLatest[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</f>
         <v>Mar. 16 - Stages Pré-After</v>
       </c>
-      <c r="M3" s="32" t="str">
+      <c r="M3" s="2" t="str">
         <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
         <v>Mar. TDS - Stages Pré-After_x000D_
-&gt; https://www.facebook.com/events/1953903148373027/1953903155039693</v>
+&gt; https://vu.fr/ndqSl</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="34">
+      <c r="A4" s="1">
         <v>45489</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="32" t="s">
         <v>291</v>
       </c>
-      <c r="C4" s="34">
+      <c r="C4" s="1">
         <v>45490</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="32" t="s">
         <v>292</v>
       </c>
       <c r="E4" s="1" t="str">
@@ -3874,7 +3864,7 @@
         <v>116</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="K4" s="2" t="str">
         <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
@@ -3887,23 +3877,23 @@
       <c r="M4" s="2" t="str">
         <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
         <v>Mar. TDS - After Mardi_x000D_
-&gt; https://www.facebook.com/events/986486549847532/986486553180865</v>
+&gt; https://vu.fr/PBIgb</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="34">
+      <c r="A5" s="1">
         <v>45490</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="32" t="s">
         <v>291</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C5" s="1">
         <v>45490</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="32" t="s">
         <v>294</v>
       </c>
       <c r="E5" s="1" t="str">
@@ -3923,7 +3913,7 @@
         <v>234</v>
       </c>
       <c r="J5" s="22" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="K5" s="2" t="str">
         <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
@@ -3936,23 +3926,23 @@
       <c r="M5" s="2" t="str">
         <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
         <v>Mer. TDS - Intensif Inter+_x000D_
-&gt; https://www.facebook.com/events/424327910394962/424327930394960</v>
+&gt; https://vu.fr/RnOqv</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="34">
+      <c r="A6" s="1">
         <v>45491</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="32" t="s">
         <v>291</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6" s="1">
         <v>45492</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="32" t="s">
         <v>292</v>
       </c>
       <c r="E6" s="1" t="str">
@@ -3972,7 +3962,7 @@
         <v>116</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="K6" s="2" t="str">
         <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
@@ -3985,24 +3975,24 @@
       <c r="M6" s="2" t="str">
         <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
         <v>Jeu. TDS - After Jeudi_x000D_
-&gt; https://www.facebook.com/events/8073251446048022/8073251459381354</v>
+&gt; https://vu.fr/OvDBA</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="34">
+      <c r="A7" s="1">
         <v>45492</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="32" t="s">
         <v>297</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="1">
         <v>45493</v>
       </c>
-      <c r="D7" s="35" t="s">
-        <v>306</v>
+      <c r="D7" s="32" t="s">
+        <v>298</v>
       </c>
       <c r="E7" s="1" t="str">
         <f>VLOOKUP(PROPER(TEXT(A7,"dddd")),TblDays[],2,FALSE)</f>
@@ -4014,44 +4004,44 @@
       <c r="G7" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="H7" s="33" t="s">
+      <c r="H7" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="I7" s="2" t="s">
         <v>109</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>299</v>
-      </c>
-      <c r="K7" s="32" t="str">
+        <v>307</v>
+      </c>
+      <c r="K7" s="2" t="str">
         <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
         <v>Ven. 🪩 Olympiades</v>
       </c>
-      <c r="L7" s="32" t="str">
+      <c r="L7" s="2" t="str">
         <f>IF(AND(TblLatest[[#This Row],[Date Fin]]&gt;TblLatest[[#This Row],[Date Début]],OR(AND(TblLatest[[#This Row],[Heure Début]]="", TblLatest[[#This Row],[Heure Fin]]=""),AND(TblLatest[[#This Row],[Date Fin]]=TblLatest[[#This Row],[Date Début]]+1,TblLatest[[#This Row],[Heure Fin]]&gt;"07h00"))), "Du " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd") &amp; " au " &amp; TEXT(TblLatest[[#This Row],[Date Fin]], "dd"), LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ". " &amp; TEXT(TblLatest[[#This Row],[Date Début]],"dd")) &amp; " - " &amp; TblLatest[[#This Row],[Nom Court]]</f>
         <v>Ven. 19 - Olympiades</v>
       </c>
-      <c r="M7" s="32" t="str">
+      <c r="M7" s="2" t="str">
         <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
         <v>Ven. Sens. Danse - Olympiades_x000D_
-&gt; https://www.facebook.com/events/981319306334689/1162077971592154/?active_tab=about</v>
+&gt; https://vu.fr/qZuKF</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="34">
+      <c r="A8" s="1">
         <v>45492</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="32" t="s">
         <v>293</v>
       </c>
-      <c r="C8" s="34">
+      <c r="C8" s="1">
         <v>45492</v>
       </c>
-      <c r="D8" s="35" t="s">
-        <v>306</v>
+      <c r="D8" s="32" t="s">
+        <v>298</v>
       </c>
       <c r="E8" s="1" t="str">
         <f>VLOOKUP(PROPER(TEXT(A8,"dddd")),TblDays[],2,FALSE)</f>
@@ -4070,7 +4060,7 @@
         <v>96</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="K8" s="2" t="str">
         <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
@@ -4083,23 +4073,23 @@
       <c r="M8" s="2" t="str">
         <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
         <v>Ven. Factory Club - Soirée RWSB_x000D_
-&gt; https://www.facebook.com/events/1144333326678800</v>
+&gt; https://vu.fr/wZdKU</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="34">
+      <c r="A9" s="1">
         <v>45493</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="32" t="s">
         <v>295</v>
       </c>
-      <c r="C9" s="34">
+      <c r="C9" s="1">
         <v>45494</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="32" t="s">
         <v>296</v>
       </c>
       <c r="E9" s="1" t="str">
@@ -4119,7 +4109,7 @@
         <v>113</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="K9" s="2" t="str">
         <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp;  " " &amp; IF(TblLatest[[#This Row],[Type]]="Evaluations","🔍",IF(TblLatest[[#This Row],[Type]]="Soirée","🪩",IF(TblLatest[[#This Row],[Type]]="Evenement","🎟️",IF(TblLatest[[#This Row],[Type]]="Stage","📚","")))) &amp; " " &amp; TblLatest[[#This Row],[Nom Court]]</f>
@@ -4132,22 +4122,22 @@
       <c r="M9" s="2" t="str">
         <f>IF(TblLatest[[#This Row],[Type]]="Evaluations",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Soirée",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".",IF(TblLatest[[#This Row],[Type]]="Evenement","WE.",IF(TblLatest[[#This Row],[Type]]="Stage",LEFT(TblLatest[[#This Row],[Jour]],3) &amp; ".","")))) &amp; " " &amp; TblLatest[[#This Row],[Lieu / Ecole]] &amp; " - " &amp; TblLatest[[#This Row],[Nom]] &amp; CHAR(13) &amp; CHAR(10) &amp; "&gt; " &amp; TblLatest[[#This Row],[URL]]</f>
         <v>Sam. Studio Diabolo - Level Up Your WCS_x000D_
-&gt; https://www.facebook.com/events/2232251107106697</v>
+&gt; https://vu.fr/Ubhqp</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J8" r:id="rId1" xr:uid="{5D73A72C-0C79-40ED-AA24-DAA42D362463}"/>
-    <hyperlink ref="J7" r:id="rId2" xr:uid="{AE43EA1E-1B17-4D9A-B614-BCD988F2CC23}"/>
-    <hyperlink ref="J2" r:id="rId3" xr:uid="{2902DCF7-845F-4874-9C1E-F291B2722CAD}"/>
-    <hyperlink ref="J3" r:id="rId4" xr:uid="{9E09D651-AF9A-49FE-82EC-8BCD8A08316A}"/>
-    <hyperlink ref="J4" r:id="rId5" xr:uid="{E1304A96-A9B1-4A2D-AE26-75A06B104C2E}"/>
-    <hyperlink ref="J5" r:id="rId6" xr:uid="{01821A44-CA7A-4496-B5C4-8C73978B7DB6}"/>
-    <hyperlink ref="J6" r:id="rId7" xr:uid="{BF2C6F75-3743-46FF-B65F-475830B50DB6}"/>
-    <hyperlink ref="J9" r:id="rId8" xr:uid="{43EE54E8-8EBF-43F6-B0AF-5F4B63DC208C}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{5C155EA5-535E-4681-A2B6-61D211E3C37E}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{B2F5D1F8-F32A-4688-815E-234CA6988D69}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{7C4D27CE-08E2-439E-97AB-7DEEA326C7B4}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{80A390EA-7E44-4AE2-A8B7-7FA19CE9265E}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{981B87B4-F45E-4492-B0EC-E0678E39A26D}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{DD487303-E530-4BE7-AA46-48270BD00932}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{3B213038-A609-4B2B-9ACC-9EAA67FC6257}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{BF80F060-7829-436A-8EB2-820B7CD24593}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>

</xml_diff>